<commit_message>
rococo.carpenter coming along well, but we have yet to fix the ExcelTableSheet.GetRow() function which needs to compare column indices with row indices
</commit_message>
<xml_diff>
--- a/tables/periodic-table.xlsx
+++ b/tables/periodic-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAA9F50-8597-417D-B75A-2567D1F89EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB83353-C7E8-4139-BC3D-CDBD4814D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sexcel-Spec" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="303">
   <si>
     <t>AtomicNumber</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Metal</t>
   </si>
   <si>
-    <t>Electronegativity</t>
-  </si>
-  <si>
     <t>FirstIonization</t>
   </si>
   <si>
@@ -848,15 +845,6 @@
     <t>C++</t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Enum</t>
-  </si>
-  <si>
-    <t>Enum-Unique</t>
-  </si>
-  <si>
     <t>Float32</t>
   </si>
   <si>
@@ -881,24 +869,15 @@
     <t>ElectronVolts</t>
   </si>
   <si>
-    <t>rococo.periodic-table.h</t>
-  </si>
-  <si>
     <t>C++ Source</t>
   </si>
   <si>
     <t>C++ Header</t>
   </si>
   <si>
-    <t>rococo.periodic-table.cpp</t>
-  </si>
-  <si>
     <t>C++ Repo</t>
   </si>
   <si>
-    <t>$(ROCOCO)tables</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
@@ -936,6 +915,36 @@
   </si>
   <si>
     <t>Define</t>
+  </si>
+  <si>
+    <t>C++ Namespace</t>
+  </si>
+  <si>
+    <t>Rococo.Science.Materials</t>
+  </si>
+  <si>
+    <t>Enum-ElementType</t>
+  </si>
+  <si>
+    <t>$(ROCOCO)</t>
+  </si>
+  <si>
+    <t>tables\rococo.periodic-table.h</t>
+  </si>
+  <si>
+    <t>tables\rococo.periodic-table.cpp</t>
+  </si>
+  <si>
+    <t>ElectroNegativity</t>
+  </si>
+  <si>
+    <t>Enum-ElementSymbol</t>
+  </si>
+  <si>
+    <t>Enum-ElementName</t>
+  </si>
+  <si>
+    <t>Int32</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1313,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" t="s">
         <v>266</v>
-      </c>
-      <c r="B1" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CE7368-B6E7-4B33-8BC2-2F805A81AC58}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1331,44 +1340,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1393,44 +1402,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" t="s">
         <v>257</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>258</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>259</v>
-      </c>
-      <c r="D1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1442,15 +1451,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3230684E-8A11-41FB-8526-9EA18FC7052C}">
   <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
@@ -1462,37 +1471,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" t="s">
         <v>270</v>
       </c>
-      <c r="B1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J1" t="s">
         <v>273</v>
       </c>
-      <c r="E1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>273</v>
-      </c>
-      <c r="H1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I1" t="s">
-        <v>273</v>
-      </c>
-      <c r="J1" t="s">
-        <v>277</v>
-      </c>
-      <c r="K1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1512,22 +1521,22 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1535,16 +1544,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>1.0069999999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>2.2000000000000002</v>
@@ -1567,16 +1576,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4">
         <v>4.0019999999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>24.587399999999999</v>
@@ -1593,19 +1602,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5">
         <v>6.9409999999999998</v>
       </c>
       <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
       </c>
       <c r="G5">
         <v>0.98</v>
@@ -1628,19 +1637,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
       <c r="D6">
         <v>9.0120000000000005</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <v>1.57</v>
@@ -1663,16 +1672,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
       </c>
       <c r="D7">
         <v>10.811</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7">
         <v>2.04</v>
@@ -1695,16 +1704,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
       </c>
       <c r="D8">
         <v>12.010999999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>2.5499999999999998</v>
@@ -1727,16 +1736,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9">
         <v>14.007</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>3.04</v>
@@ -1759,16 +1768,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
       </c>
       <c r="D10">
         <v>15.999000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>3.44</v>
@@ -1791,16 +1800,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
       <c r="D11">
         <v>18.998000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11">
         <v>3.98</v>
@@ -1823,16 +1832,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
       </c>
       <c r="D12">
         <v>20.18</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12">
         <v>21.564499999999999</v>
@@ -1852,19 +1861,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
       <c r="D13">
         <v>22.99</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
         <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
       </c>
       <c r="G13">
         <v>0.93</v>
@@ -1887,19 +1896,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
       <c r="D14">
         <v>24.305</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>1.31</v>
@@ -1922,16 +1931,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
       </c>
       <c r="D15">
         <v>26.981999999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -1957,16 +1966,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
       </c>
       <c r="D16">
         <v>28.085999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <v>1.9</v>
@@ -1989,16 +1998,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
       </c>
       <c r="D17">
         <v>30.974</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>2.19</v>
@@ -2021,16 +2030,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
       <c r="D18">
         <v>32.064999999999998</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <v>2.58</v>
@@ -2053,16 +2062,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
       </c>
       <c r="D19">
         <v>35.453000000000003</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19">
         <v>3.16</v>
@@ -2085,16 +2094,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
       </c>
       <c r="D20">
         <v>39.948</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20">
         <v>15.759600000000001</v>
@@ -2114,19 +2123,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
       </c>
       <c r="D21">
         <v>39.097999999999999</v>
       </c>
       <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
         <v>18</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
       </c>
       <c r="G21">
         <v>0.82</v>
@@ -2149,19 +2158,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
       </c>
       <c r="D22">
         <v>40.078000000000003</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2184,19 +2193,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
       </c>
       <c r="D23">
         <v>44.956000000000003</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23">
         <v>1.36</v>
@@ -2219,19 +2228,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
       </c>
       <c r="D24">
         <v>47.866999999999997</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24">
         <v>1.54</v>
@@ -2254,19 +2263,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
         <v>62</v>
-      </c>
-      <c r="C25" t="s">
-        <v>63</v>
       </c>
       <c r="D25">
         <v>50.942</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25">
         <v>1.63</v>
@@ -2289,19 +2298,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
         <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
       </c>
       <c r="D26">
         <v>51.996000000000002</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26">
         <v>1.66</v>
@@ -2324,19 +2333,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
       </c>
       <c r="D27">
         <v>54.938000000000002</v>
       </c>
       <c r="E27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27">
         <v>1.55</v>
@@ -2359,19 +2368,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
       </c>
       <c r="D28">
         <v>55.844999999999999</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28">
         <v>1.83</v>
@@ -2394,19 +2403,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" t="s">
-        <v>71</v>
       </c>
       <c r="D29">
         <v>58.933</v>
       </c>
       <c r="E29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29">
         <v>1.88</v>
@@ -2429,19 +2438,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
       </c>
       <c r="D30">
         <v>58.692999999999998</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30">
         <v>1.91</v>
@@ -2464,19 +2473,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
         <v>74</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
       </c>
       <c r="D31">
         <v>63.545999999999999</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31">
         <v>1.9</v>
@@ -2499,19 +2508,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" t="s">
-        <v>77</v>
       </c>
       <c r="D32">
         <v>65.38</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32">
         <v>1.65</v>
@@ -2534,16 +2543,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
         <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>79</v>
       </c>
       <c r="D33">
         <v>69.722999999999999</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
         <v>4</v>
@@ -2569,16 +2578,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
         <v>80</v>
-      </c>
-      <c r="C34" t="s">
-        <v>81</v>
       </c>
       <c r="D34">
         <v>72.64</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G34">
         <v>2.0099999999999998</v>
@@ -2601,16 +2610,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" t="s">
         <v>82</v>
-      </c>
-      <c r="C35" t="s">
-        <v>83</v>
       </c>
       <c r="D35">
         <v>74.921999999999997</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G35">
         <v>2.1800000000000002</v>
@@ -2633,16 +2642,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
         <v>84</v>
-      </c>
-      <c r="C36" t="s">
-        <v>85</v>
       </c>
       <c r="D36">
         <v>78.959999999999994</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36">
         <v>2.5499999999999998</v>
@@ -2665,16 +2674,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
         <v>86</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
       </c>
       <c r="D37">
         <v>79.903999999999996</v>
       </c>
       <c r="F37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G37">
         <v>2.96</v>
@@ -2697,16 +2706,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" t="s">
         <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>89</v>
       </c>
       <c r="D38">
         <v>83.798000000000002</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38">
         <v>13.999599999999999</v>
@@ -2726,19 +2735,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
         <v>90</v>
-      </c>
-      <c r="C39" t="s">
-        <v>91</v>
       </c>
       <c r="D39">
         <v>85.468000000000004</v>
       </c>
       <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
         <v>18</v>
-      </c>
-      <c r="F39" t="s">
-        <v>19</v>
       </c>
       <c r="G39">
         <v>0.82</v>
@@ -2761,19 +2770,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s">
         <v>92</v>
-      </c>
-      <c r="C40" t="s">
-        <v>93</v>
       </c>
       <c r="D40">
         <v>87.62</v>
       </c>
       <c r="E40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40">
         <v>0.95</v>
@@ -2796,19 +2805,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" t="s">
         <v>94</v>
-      </c>
-      <c r="C41" t="s">
-        <v>95</v>
       </c>
       <c r="D41">
         <v>88.906000000000006</v>
       </c>
       <c r="E41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G41">
         <v>1.22</v>
@@ -2831,19 +2840,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
         <v>96</v>
-      </c>
-      <c r="C42" t="s">
-        <v>97</v>
       </c>
       <c r="D42">
         <v>91.224000000000004</v>
       </c>
       <c r="E42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G42">
         <v>1.33</v>
@@ -2866,19 +2875,19 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
         <v>98</v>
-      </c>
-      <c r="C43" t="s">
-        <v>99</v>
       </c>
       <c r="D43">
         <v>92.906000000000006</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G43">
         <v>1.6</v>
@@ -2901,19 +2910,19 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" t="s">
         <v>100</v>
-      </c>
-      <c r="C44" t="s">
-        <v>101</v>
       </c>
       <c r="D44">
         <v>95.96</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G44">
         <v>2.16</v>
@@ -2936,19 +2945,19 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
         <v>102</v>
-      </c>
-      <c r="C45" t="s">
-        <v>103</v>
       </c>
       <c r="D45">
         <v>98</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G45">
         <v>1.9</v>
@@ -2971,19 +2980,19 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s">
         <v>104</v>
-      </c>
-      <c r="C46" t="s">
-        <v>105</v>
       </c>
       <c r="D46">
         <v>101.07</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G46">
         <v>2.2000000000000002</v>
@@ -3006,19 +3015,19 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
         <v>106</v>
-      </c>
-      <c r="C47" t="s">
-        <v>107</v>
       </c>
       <c r="D47">
         <v>102.90600000000001</v>
       </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G47">
         <v>2.2799999999999998</v>
@@ -3041,19 +3050,19 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s">
         <v>108</v>
-      </c>
-      <c r="C48" t="s">
-        <v>109</v>
       </c>
       <c r="D48">
         <v>106.42</v>
       </c>
       <c r="E48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G48">
         <v>2.2000000000000002</v>
@@ -3076,19 +3085,19 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" t="s">
         <v>110</v>
-      </c>
-      <c r="C49" t="s">
-        <v>111</v>
       </c>
       <c r="D49">
         <v>107.86799999999999</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G49">
         <v>1.93</v>
@@ -3111,19 +3120,19 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
         <v>112</v>
-      </c>
-      <c r="C50" t="s">
-        <v>113</v>
       </c>
       <c r="D50">
         <v>112.411</v>
       </c>
       <c r="E50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G50">
         <v>1.69</v>
@@ -3146,16 +3155,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
         <v>114</v>
-      </c>
-      <c r="C51" t="s">
-        <v>115</v>
       </c>
       <c r="D51">
         <v>114.818</v>
       </c>
       <c r="E51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F51" t="s">
         <v>4</v>
@@ -3181,16 +3190,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" t="s">
         <v>116</v>
-      </c>
-      <c r="C52" t="s">
-        <v>117</v>
       </c>
       <c r="D52">
         <v>118.71</v>
       </c>
       <c r="E52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F52" t="s">
         <v>4</v>
@@ -3216,16 +3225,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
         <v>118</v>
-      </c>
-      <c r="C53" t="s">
-        <v>119</v>
       </c>
       <c r="D53">
         <v>121.76</v>
       </c>
       <c r="F53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G53">
         <v>2.0499999999999998</v>
@@ -3248,16 +3257,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
         <v>120</v>
-      </c>
-      <c r="C54" t="s">
-        <v>121</v>
       </c>
       <c r="D54">
         <v>127.6</v>
       </c>
       <c r="F54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G54">
         <v>2.1</v>
@@ -3280,16 +3289,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
         <v>122</v>
-      </c>
-      <c r="C55" t="s">
-        <v>123</v>
       </c>
       <c r="D55">
         <v>126.904</v>
       </c>
       <c r="F55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G55">
         <v>2.66</v>
@@ -3312,16 +3321,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
         <v>124</v>
-      </c>
-      <c r="C56" t="s">
-        <v>125</v>
       </c>
       <c r="D56">
         <v>131.29300000000001</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56">
         <v>12.129799999999999</v>
@@ -3341,19 +3350,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s">
         <v>126</v>
-      </c>
-      <c r="C57" t="s">
-        <v>127</v>
       </c>
       <c r="D57">
         <v>132.905</v>
       </c>
       <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
         <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>19</v>
       </c>
       <c r="G57">
         <v>0.79</v>
@@ -3376,19 +3385,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
         <v>128</v>
-      </c>
-      <c r="C58" t="s">
-        <v>129</v>
       </c>
       <c r="D58">
         <v>137.327</v>
       </c>
       <c r="E58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G58">
         <v>0.89</v>
@@ -3411,19 +3420,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" t="s">
         <v>130</v>
-      </c>
-      <c r="C59" t="s">
-        <v>131</v>
       </c>
       <c r="D59">
         <v>138.905</v>
       </c>
       <c r="E59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G59">
         <v>1.1000000000000001</v>
@@ -3446,19 +3455,19 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" t="s">
         <v>133</v>
-      </c>
-      <c r="C60" t="s">
-        <v>134</v>
       </c>
       <c r="D60">
         <v>140.11600000000001</v>
       </c>
       <c r="E60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G60">
         <v>1.1200000000000001</v>
@@ -3481,19 +3490,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" t="s">
         <v>135</v>
-      </c>
-      <c r="C61" t="s">
-        <v>136</v>
       </c>
       <c r="D61">
         <v>140.90799999999999</v>
       </c>
       <c r="E61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G61">
         <v>1.1299999999999999</v>
@@ -3516,19 +3525,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" t="s">
         <v>137</v>
-      </c>
-      <c r="C62" t="s">
-        <v>138</v>
       </c>
       <c r="D62">
         <v>144.24199999999999</v>
       </c>
       <c r="E62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G62">
         <v>1.1399999999999999</v>
@@ -3551,19 +3560,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" t="s">
         <v>139</v>
-      </c>
-      <c r="C63" t="s">
-        <v>140</v>
       </c>
       <c r="D63">
         <v>145</v>
       </c>
       <c r="E63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G63">
         <v>1.1299999999999999</v>
@@ -3586,19 +3595,19 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
         <v>141</v>
-      </c>
-      <c r="C64" t="s">
-        <v>142</v>
       </c>
       <c r="D64">
         <v>150.36000000000001</v>
       </c>
       <c r="E64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G64">
         <v>1.17</v>
@@ -3621,19 +3630,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" t="s">
         <v>143</v>
-      </c>
-      <c r="C65" t="s">
-        <v>144</v>
       </c>
       <c r="D65">
         <v>151.964</v>
       </c>
       <c r="E65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G65">
         <v>1.2</v>
@@ -3656,19 +3665,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" t="s">
         <v>145</v>
-      </c>
-      <c r="C66" t="s">
-        <v>146</v>
       </c>
       <c r="D66">
         <v>157.25</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G66">
         <v>1.2</v>
@@ -3691,19 +3700,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" t="s">
         <v>147</v>
-      </c>
-      <c r="C67" t="s">
-        <v>148</v>
       </c>
       <c r="D67">
         <v>158.92500000000001</v>
       </c>
       <c r="E67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G67">
         <v>1.2</v>
@@ -3726,19 +3735,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" t="s">
         <v>149</v>
-      </c>
-      <c r="C68" t="s">
-        <v>150</v>
       </c>
       <c r="D68">
         <v>162.5</v>
       </c>
       <c r="E68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G68">
         <v>1.22</v>
@@ -3761,19 +3770,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" t="s">
         <v>151</v>
-      </c>
-      <c r="C69" t="s">
-        <v>152</v>
       </c>
       <c r="D69">
         <v>164.93</v>
       </c>
       <c r="E69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G69">
         <v>1.23</v>
@@ -3796,19 +3805,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" t="s">
         <v>153</v>
-      </c>
-      <c r="C70" t="s">
-        <v>154</v>
       </c>
       <c r="D70">
         <v>167.25899999999999</v>
       </c>
       <c r="E70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G70">
         <v>1.24</v>
@@ -3831,19 +3840,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" t="s">
         <v>155</v>
-      </c>
-      <c r="C71" t="s">
-        <v>156</v>
       </c>
       <c r="D71">
         <v>168.934</v>
       </c>
       <c r="E71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G71">
         <v>1.25</v>
@@ -3866,19 +3875,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" t="s">
         <v>157</v>
-      </c>
-      <c r="C72" t="s">
-        <v>158</v>
       </c>
       <c r="D72">
         <v>173.054</v>
       </c>
       <c r="E72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G72">
         <v>1.1000000000000001</v>
@@ -3901,19 +3910,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" t="s">
         <v>159</v>
-      </c>
-      <c r="C73" t="s">
-        <v>160</v>
       </c>
       <c r="D73">
         <v>174.96700000000001</v>
       </c>
       <c r="E73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G73">
         <v>1.27</v>
@@ -3936,19 +3945,19 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="s">
         <v>161</v>
-      </c>
-      <c r="C74" t="s">
-        <v>162</v>
       </c>
       <c r="D74">
         <v>178.49</v>
       </c>
       <c r="E74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G74">
         <v>1.3</v>
@@ -3971,19 +3980,19 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>162</v>
+      </c>
+      <c r="C75" t="s">
         <v>163</v>
-      </c>
-      <c r="C75" t="s">
-        <v>164</v>
       </c>
       <c r="D75">
         <v>180.94800000000001</v>
       </c>
       <c r="E75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G75">
         <v>1.5</v>
@@ -4006,19 +4015,19 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" t="s">
         <v>165</v>
-      </c>
-      <c r="C76" t="s">
-        <v>166</v>
       </c>
       <c r="D76">
         <v>183.84</v>
       </c>
       <c r="E76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G76">
         <v>2.36</v>
@@ -4041,19 +4050,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>166</v>
+      </c>
+      <c r="C77" t="s">
         <v>167</v>
-      </c>
-      <c r="C77" t="s">
-        <v>168</v>
       </c>
       <c r="D77">
         <v>186.20699999999999</v>
       </c>
       <c r="E77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G77">
         <v>1.9</v>
@@ -4076,19 +4085,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" t="s">
         <v>169</v>
-      </c>
-      <c r="C78" t="s">
-        <v>170</v>
       </c>
       <c r="D78">
         <v>190.23</v>
       </c>
       <c r="E78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G78">
         <v>2.2000000000000002</v>
@@ -4111,19 +4120,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" t="s">
         <v>171</v>
-      </c>
-      <c r="C79" t="s">
-        <v>172</v>
       </c>
       <c r="D79">
         <v>192.21700000000001</v>
       </c>
       <c r="E79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G79">
         <v>2.2000000000000002</v>
@@ -4146,19 +4155,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
+        <v>172</v>
+      </c>
+      <c r="C80" t="s">
         <v>173</v>
-      </c>
-      <c r="C80" t="s">
-        <v>174</v>
       </c>
       <c r="D80">
         <v>195.084</v>
       </c>
       <c r="E80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G80">
         <v>2.2799999999999998</v>
@@ -4181,19 +4190,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" t="s">
         <v>175</v>
-      </c>
-      <c r="C81" t="s">
-        <v>176</v>
       </c>
       <c r="D81">
         <v>196.96700000000001</v>
       </c>
       <c r="E81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G81">
         <v>2.54</v>
@@ -4216,19 +4225,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" t="s">
         <v>177</v>
-      </c>
-      <c r="C82" t="s">
-        <v>178</v>
       </c>
       <c r="D82">
         <v>200.59</v>
       </c>
       <c r="E82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G82">
         <v>2</v>
@@ -4251,16 +4260,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" t="s">
         <v>179</v>
-      </c>
-      <c r="C83" t="s">
-        <v>180</v>
       </c>
       <c r="D83">
         <v>204.38300000000001</v>
       </c>
       <c r="E83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F83" t="s">
         <v>4</v>
@@ -4286,16 +4295,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" t="s">
         <v>181</v>
-      </c>
-      <c r="C84" t="s">
-        <v>182</v>
       </c>
       <c r="D84">
         <v>207.2</v>
       </c>
       <c r="E84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F84" t="s">
         <v>4</v>
@@ -4321,16 +4330,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" t="s">
         <v>183</v>
-      </c>
-      <c r="C85" t="s">
-        <v>184</v>
       </c>
       <c r="D85">
         <v>208.98</v>
       </c>
       <c r="E85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F85" t="s">
         <v>4</v>
@@ -4356,16 +4365,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>184</v>
+      </c>
+      <c r="C86" t="s">
         <v>185</v>
-      </c>
-      <c r="C86" t="s">
-        <v>186</v>
       </c>
       <c r="D86">
         <v>210</v>
       </c>
       <c r="F86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G86">
         <v>2</v>
@@ -4388,16 +4397,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" t="s">
         <v>187</v>
-      </c>
-      <c r="C87" t="s">
-        <v>188</v>
       </c>
       <c r="D87">
         <v>210</v>
       </c>
       <c r="F87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G87">
         <v>2.2000000000000002</v>
@@ -4420,19 +4429,19 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" t="s">
         <v>189</v>
-      </c>
-      <c r="C88" t="s">
-        <v>190</v>
       </c>
       <c r="D88">
         <v>222</v>
       </c>
       <c r="E88" t="s">
+        <v>17</v>
+      </c>
+      <c r="F88" t="s">
         <v>18</v>
-      </c>
-      <c r="F88" t="s">
-        <v>19</v>
       </c>
       <c r="H88">
         <v>10.7485</v>
@@ -4452,19 +4461,19 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
+        <v>190</v>
+      </c>
+      <c r="C89" t="s">
         <v>191</v>
-      </c>
-      <c r="C89" t="s">
-        <v>192</v>
       </c>
       <c r="D89">
         <v>223</v>
       </c>
       <c r="E89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G89">
         <v>0.7</v>
@@ -4487,19 +4496,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
+        <v>192</v>
+      </c>
+      <c r="C90" t="s">
         <v>193</v>
-      </c>
-      <c r="C90" t="s">
-        <v>194</v>
       </c>
       <c r="D90">
         <v>226</v>
       </c>
       <c r="E90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G90">
         <v>0.9</v>
@@ -4522,19 +4531,19 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
+        <v>195</v>
+      </c>
+      <c r="C91" t="s">
         <v>196</v>
-      </c>
-      <c r="C91" t="s">
-        <v>197</v>
       </c>
       <c r="D91">
         <v>227</v>
       </c>
       <c r="E91" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F91" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G91">
         <v>1.1000000000000001</v>
@@ -4557,19 +4566,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" t="s">
         <v>198</v>
-      </c>
-      <c r="C92" t="s">
-        <v>199</v>
       </c>
       <c r="D92">
         <v>232.03800000000001</v>
       </c>
       <c r="E92" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F92" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G92">
         <v>1.3</v>
@@ -4592,19 +4601,19 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
+        <v>199</v>
+      </c>
+      <c r="C93" t="s">
         <v>200</v>
-      </c>
-      <c r="C93" t="s">
-        <v>201</v>
       </c>
       <c r="D93">
         <v>231.036</v>
       </c>
       <c r="E93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G93">
         <v>1.5</v>
@@ -4627,19 +4636,19 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
+        <v>201</v>
+      </c>
+      <c r="C94" t="s">
         <v>202</v>
-      </c>
-      <c r="C94" t="s">
-        <v>203</v>
       </c>
       <c r="D94">
         <v>238.029</v>
       </c>
       <c r="E94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G94">
         <v>1.38</v>
@@ -4662,19 +4671,19 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
+        <v>203</v>
+      </c>
+      <c r="C95" t="s">
         <v>204</v>
-      </c>
-      <c r="C95" t="s">
-        <v>205</v>
       </c>
       <c r="D95">
         <v>237</v>
       </c>
       <c r="E95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F95" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G95">
         <v>1.36</v>
@@ -4697,19 +4706,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
+        <v>205</v>
+      </c>
+      <c r="C96" t="s">
         <v>206</v>
-      </c>
-      <c r="C96" t="s">
-        <v>207</v>
       </c>
       <c r="D96">
         <v>244</v>
       </c>
       <c r="E96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F96" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G96">
         <v>1.28</v>
@@ -4732,19 +4741,19 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>207</v>
+      </c>
+      <c r="C97" t="s">
         <v>208</v>
-      </c>
-      <c r="C97" t="s">
-        <v>209</v>
       </c>
       <c r="D97">
         <v>243</v>
       </c>
       <c r="E97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F97" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G97">
         <v>1.3</v>
@@ -4767,19 +4776,19 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" t="s">
         <v>210</v>
-      </c>
-      <c r="C98" t="s">
-        <v>211</v>
       </c>
       <c r="D98">
         <v>247</v>
       </c>
       <c r="E98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F98" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G98">
         <v>1.3</v>
@@ -4802,19 +4811,19 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
+        <v>211</v>
+      </c>
+      <c r="C99" t="s">
         <v>212</v>
-      </c>
-      <c r="C99" t="s">
-        <v>213</v>
       </c>
       <c r="D99">
         <v>247</v>
       </c>
       <c r="E99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G99">
         <v>1.3</v>
@@ -4837,19 +4846,19 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>213</v>
+      </c>
+      <c r="C100" t="s">
         <v>214</v>
-      </c>
-      <c r="C100" t="s">
-        <v>215</v>
       </c>
       <c r="D100">
         <v>251</v>
       </c>
       <c r="E100" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F100" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G100">
         <v>1.3</v>
@@ -4872,19 +4881,19 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>215</v>
+      </c>
+      <c r="C101" t="s">
         <v>216</v>
-      </c>
-      <c r="C101" t="s">
-        <v>217</v>
       </c>
       <c r="D101">
         <v>252</v>
       </c>
       <c r="E101" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G101">
         <v>1.3</v>
@@ -4904,19 +4913,19 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
+        <v>217</v>
+      </c>
+      <c r="C102" t="s">
         <v>218</v>
-      </c>
-      <c r="C102" t="s">
-        <v>219</v>
       </c>
       <c r="D102">
         <v>257</v>
       </c>
       <c r="E102" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F102" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G102">
         <v>1.3</v>
@@ -4930,19 +4939,19 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
+        <v>219</v>
+      </c>
+      <c r="C103" t="s">
         <v>220</v>
-      </c>
-      <c r="C103" t="s">
-        <v>221</v>
       </c>
       <c r="D103">
         <v>258</v>
       </c>
       <c r="E103" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G103">
         <v>1.3</v>
@@ -4956,19 +4965,19 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
+        <v>221</v>
+      </c>
+      <c r="C104" t="s">
         <v>222</v>
-      </c>
-      <c r="C104" t="s">
-        <v>223</v>
       </c>
       <c r="D104">
         <v>259</v>
       </c>
       <c r="E104" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G104">
         <v>1.3</v>
@@ -4982,19 +4991,19 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
+        <v>223</v>
+      </c>
+      <c r="C105" t="s">
         <v>224</v>
-      </c>
-      <c r="C105" t="s">
-        <v>225</v>
       </c>
       <c r="D105">
         <v>262</v>
       </c>
       <c r="E105" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F105" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -5002,19 +5011,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
+        <v>225</v>
+      </c>
+      <c r="C106" t="s">
         <v>226</v>
-      </c>
-      <c r="C106" t="s">
-        <v>227</v>
       </c>
       <c r="D106">
         <v>261</v>
       </c>
       <c r="E106" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F106" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I106" s="1">
         <v>18.100000000000001</v>
@@ -5025,19 +5034,19 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" t="s">
         <v>229</v>
-      </c>
-      <c r="C107" t="s">
-        <v>230</v>
       </c>
       <c r="D107">
         <v>262</v>
       </c>
       <c r="E107" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I107" s="1">
         <v>39</v>
@@ -5048,19 +5057,19 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
+        <v>230</v>
+      </c>
+      <c r="C108" t="s">
         <v>231</v>
-      </c>
-      <c r="C108" t="s">
-        <v>232</v>
       </c>
       <c r="D108">
         <v>266</v>
       </c>
       <c r="E108" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I108" s="1">
         <v>35</v>
@@ -5071,19 +5080,19 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
+        <v>232</v>
+      </c>
+      <c r="C109" t="s">
         <v>233</v>
-      </c>
-      <c r="C109" t="s">
-        <v>234</v>
       </c>
       <c r="D109">
         <v>264</v>
       </c>
       <c r="E109" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I109" s="1">
         <v>37</v>
@@ -5094,19 +5103,19 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
+        <v>234</v>
+      </c>
+      <c r="C110" t="s">
         <v>235</v>
-      </c>
-      <c r="C110" t="s">
-        <v>236</v>
       </c>
       <c r="D110">
         <v>267</v>
       </c>
       <c r="E110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F110" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I110" s="1">
         <v>41</v>
@@ -5117,19 +5126,19 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
+        <v>236</v>
+      </c>
+      <c r="C111" t="s">
         <v>237</v>
-      </c>
-      <c r="C111" t="s">
-        <v>238</v>
       </c>
       <c r="D111">
         <v>268</v>
       </c>
       <c r="E111" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F111" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I111" s="1">
         <v>35</v>
@@ -5140,19 +5149,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
+        <v>238</v>
+      </c>
+      <c r="C112" t="s">
         <v>239</v>
-      </c>
-      <c r="C112" t="s">
-        <v>240</v>
       </c>
       <c r="D112">
         <v>271</v>
       </c>
       <c r="E112" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F112" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -5160,19 +5169,19 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
+        <v>240</v>
+      </c>
+      <c r="C113" t="s">
         <v>241</v>
-      </c>
-      <c r="C113" t="s">
-        <v>242</v>
       </c>
       <c r="D113">
         <v>272</v>
       </c>
       <c r="E113" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F113" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -5180,19 +5189,19 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
+        <v>242</v>
+      </c>
+      <c r="C114" t="s">
         <v>243</v>
-      </c>
-      <c r="C114" t="s">
-        <v>244</v>
       </c>
       <c r="D114">
         <v>285</v>
       </c>
       <c r="E114" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F114" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -5200,16 +5209,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
+        <v>244</v>
+      </c>
+      <c r="C115" t="s">
         <v>245</v>
-      </c>
-      <c r="C115" t="s">
-        <v>246</v>
       </c>
       <c r="D115">
         <v>284</v>
       </c>
       <c r="E115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -5217,19 +5226,19 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
+        <v>246</v>
+      </c>
+      <c r="C116" t="s">
         <v>247</v>
-      </c>
-      <c r="C116" t="s">
-        <v>248</v>
       </c>
       <c r="D116">
         <v>289</v>
       </c>
       <c r="E116" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F116" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -5237,16 +5246,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
+        <v>248</v>
+      </c>
+      <c r="C117" t="s">
         <v>249</v>
-      </c>
-      <c r="C117" t="s">
-        <v>250</v>
       </c>
       <c r="D117">
         <v>288</v>
       </c>
       <c r="E117" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -5254,19 +5263,19 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
+        <v>250</v>
+      </c>
+      <c r="C118" t="s">
         <v>251</v>
-      </c>
-      <c r="C118" t="s">
-        <v>252</v>
       </c>
       <c r="D118">
         <v>292</v>
       </c>
       <c r="E118" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -5274,10 +5283,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
+        <v>252</v>
+      </c>
+      <c r="C119" t="s">
         <v>253</v>
-      </c>
-      <c r="C119" t="s">
-        <v>254</v>
       </c>
       <c r="D119">
         <v>295</v>
@@ -5288,16 +5297,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
+        <v>254</v>
+      </c>
+      <c r="C120" t="s">
         <v>255</v>
-      </c>
-      <c r="C120" t="s">
-        <v>256</v>
       </c>
       <c r="D120">
         <v>294</v>
       </c>
       <c r="F120" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5311,10 +5320,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5327,71 +5336,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" t="s">
         <v>268</v>
-      </c>
-      <c r="B1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented table generation in rococo.carpenter. The element table looks correct, but is untestsed. Todo: test the element table, build an excel template and try out on more tables.
</commit_message>
<xml_diff>
--- a/tables/periodic-table.xlsx
+++ b/tables/periodic-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB83353-C7E8-4139-BC3D-CDBD4814D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD4F0AC-2668-437C-A450-7A08601455A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="302">
   <si>
     <t>AtomicNumber</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Li</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Alkali Metal</t>
@@ -1313,10 +1310,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
         <v>265</v>
-      </c>
-      <c r="B1" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -1340,44 +1337,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" t="s">
         <v>286</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>287</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>288</v>
-      </c>
-      <c r="E1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" t="s">
         <v>275</v>
       </c>
-      <c r="C3" t="s">
-        <v>276</v>
-      </c>
       <c r="D3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1402,44 +1399,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" t="s">
         <v>256</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>257</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>258</v>
-      </c>
-      <c r="D1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1452,7 +1449,7 @@
   <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,37 +1468,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
         <v>269</v>
       </c>
-      <c r="E1" t="s">
-        <v>270</v>
-      </c>
       <c r="F1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1521,10 +1518,10 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -1551,6 +1548,9 @@
       </c>
       <c r="D3">
         <v>1.0069999999999999</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1584,6 +1584,9 @@
       <c r="D4">
         <v>4.0019999999999998</v>
       </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -1610,11 +1613,11 @@
       <c r="D5">
         <v>6.9409999999999998</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
       </c>
       <c r="G5">
         <v>0.98</v>
@@ -1637,19 +1640,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
       <c r="D6">
         <v>9.0120000000000005</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
+      <c r="E6" t="b">
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>1.57</v>
@@ -1672,16 +1675,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
       </c>
       <c r="D7">
         <v>10.811</v>
       </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>2.04</v>
@@ -1704,13 +1710,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
       <c r="D8">
         <v>12.010999999999999</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -1736,13 +1745,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9">
         <v>14.007</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -1768,13 +1780,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
       </c>
       <c r="D10">
         <v>15.999000000000001</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -1800,16 +1815,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
       <c r="D11">
         <v>18.998000000000001</v>
       </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11">
         <v>3.98</v>
@@ -1832,13 +1850,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
       <c r="D12">
         <v>20.18</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -1861,19 +1882,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
       <c r="D13">
         <v>22.99</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
       </c>
       <c r="G13">
         <v>0.93</v>
@@ -1896,19 +1917,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
       </c>
       <c r="D14">
         <v>24.305</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
+      <c r="E14" t="b">
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14">
         <v>1.31</v>
@@ -1931,16 +1952,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
       </c>
       <c r="D15">
         <v>26.981999999999999</v>
       </c>
-      <c r="E15" t="s">
-        <v>17</v>
+      <c r="E15" t="b">
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -1966,16 +1987,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
       </c>
       <c r="D16">
         <v>28.085999999999999</v>
       </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16">
         <v>1.9</v>
@@ -1998,13 +2022,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
       <c r="D17">
         <v>30.974</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -2030,13 +2057,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
       </c>
       <c r="D18">
         <v>32.064999999999998</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -2062,16 +2092,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
         <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
       </c>
       <c r="D19">
         <v>35.453000000000003</v>
       </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19">
         <v>3.16</v>
@@ -2094,13 +2127,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
       </c>
       <c r="D20">
         <v>39.948</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -2123,19 +2159,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
       </c>
       <c r="D21">
         <v>39.097999999999999</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
       </c>
       <c r="G21">
         <v>0.82</v>
@@ -2158,19 +2194,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
       </c>
       <c r="D22">
         <v>40.078000000000003</v>
       </c>
-      <c r="E22" t="s">
-        <v>17</v>
+      <c r="E22" t="b">
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2193,19 +2229,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
       </c>
       <c r="D23">
         <v>44.956000000000003</v>
       </c>
-      <c r="E23" t="s">
-        <v>17</v>
+      <c r="E23" t="b">
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23">
         <v>1.36</v>
@@ -2228,19 +2264,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
         <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
       </c>
       <c r="D24">
         <v>47.866999999999997</v>
       </c>
-      <c r="E24" t="s">
-        <v>17</v>
+      <c r="E24" t="b">
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24">
         <v>1.54</v>
@@ -2263,19 +2299,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
         <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
       </c>
       <c r="D25">
         <v>50.942</v>
       </c>
-      <c r="E25" t="s">
-        <v>17</v>
+      <c r="E25" t="b">
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25">
         <v>1.63</v>
@@ -2298,19 +2334,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
       </c>
       <c r="D26">
         <v>51.996000000000002</v>
       </c>
-      <c r="E26" t="s">
-        <v>17</v>
+      <c r="E26" t="b">
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26">
         <v>1.66</v>
@@ -2333,19 +2369,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
         <v>65</v>
-      </c>
-      <c r="C27" t="s">
-        <v>66</v>
       </c>
       <c r="D27">
         <v>54.938000000000002</v>
       </c>
-      <c r="E27" t="s">
-        <v>17</v>
+      <c r="E27" t="b">
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27">
         <v>1.55</v>
@@ -2368,19 +2404,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
         <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
       </c>
       <c r="D28">
         <v>55.844999999999999</v>
       </c>
-      <c r="E28" t="s">
-        <v>17</v>
+      <c r="E28" t="b">
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G28">
         <v>1.83</v>
@@ -2403,19 +2439,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
         <v>69</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
       </c>
       <c r="D29">
         <v>58.933</v>
       </c>
-      <c r="E29" t="s">
-        <v>17</v>
+      <c r="E29" t="b">
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29">
         <v>1.88</v>
@@ -2438,19 +2474,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
         <v>71</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
       </c>
       <c r="D30">
         <v>58.692999999999998</v>
       </c>
-      <c r="E30" t="s">
-        <v>17</v>
+      <c r="E30" t="b">
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30">
         <v>1.91</v>
@@ -2473,19 +2509,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
       </c>
       <c r="D31">
         <v>63.545999999999999</v>
       </c>
-      <c r="E31" t="s">
-        <v>17</v>
+      <c r="E31" t="b">
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G31">
         <v>1.9</v>
@@ -2508,19 +2544,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
         <v>75</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
       </c>
       <c r="D32">
         <v>65.38</v>
       </c>
-      <c r="E32" t="s">
-        <v>17</v>
+      <c r="E32" t="b">
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G32">
         <v>1.65</v>
@@ -2543,16 +2579,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
         <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
       </c>
       <c r="D33">
         <v>69.722999999999999</v>
       </c>
-      <c r="E33" t="s">
-        <v>17</v>
+      <c r="E33" t="b">
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>4</v>
@@ -2578,16 +2614,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
         <v>79</v>
-      </c>
-      <c r="C34" t="s">
-        <v>80</v>
       </c>
       <c r="D34">
         <v>72.64</v>
       </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
       <c r="F34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>2.0099999999999998</v>
@@ -2610,16 +2649,19 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
         <v>81</v>
-      </c>
-      <c r="C35" t="s">
-        <v>82</v>
       </c>
       <c r="D35">
         <v>74.921999999999997</v>
       </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
       <c r="F35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35">
         <v>2.1800000000000002</v>
@@ -2642,13 +2684,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
         <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>84</v>
       </c>
       <c r="D36">
         <v>78.959999999999994</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -2674,16 +2719,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
         <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
       </c>
       <c r="D37">
         <v>79.903999999999996</v>
       </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G37">
         <v>2.96</v>
@@ -2706,13 +2754,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
         <v>87</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
       </c>
       <c r="D38">
         <v>83.798000000000002</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -2735,19 +2786,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
         <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>90</v>
       </c>
       <c r="D39">
         <v>85.468000000000004</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>17</v>
-      </c>
-      <c r="F39" t="s">
-        <v>18</v>
       </c>
       <c r="G39">
         <v>0.82</v>
@@ -2770,19 +2821,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
         <v>91</v>
-      </c>
-      <c r="C40" t="s">
-        <v>92</v>
       </c>
       <c r="D40">
         <v>87.62</v>
       </c>
-      <c r="E40" t="s">
-        <v>17</v>
+      <c r="E40" t="b">
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40">
         <v>0.95</v>
@@ -2805,19 +2856,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" t="s">
         <v>93</v>
-      </c>
-      <c r="C41" t="s">
-        <v>94</v>
       </c>
       <c r="D41">
         <v>88.906000000000006</v>
       </c>
-      <c r="E41" t="s">
-        <v>17</v>
+      <c r="E41" t="b">
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G41">
         <v>1.22</v>
@@ -2840,19 +2891,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" t="s">
         <v>95</v>
-      </c>
-      <c r="C42" t="s">
-        <v>96</v>
       </c>
       <c r="D42">
         <v>91.224000000000004</v>
       </c>
-      <c r="E42" t="s">
-        <v>17</v>
+      <c r="E42" t="b">
+        <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G42">
         <v>1.33</v>
@@ -2875,19 +2926,19 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s">
         <v>97</v>
-      </c>
-      <c r="C43" t="s">
-        <v>98</v>
       </c>
       <c r="D43">
         <v>92.906000000000006</v>
       </c>
-      <c r="E43" t="s">
-        <v>17</v>
+      <c r="E43" t="b">
+        <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G43">
         <v>1.6</v>
@@ -2910,19 +2961,19 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" t="s">
         <v>99</v>
-      </c>
-      <c r="C44" t="s">
-        <v>100</v>
       </c>
       <c r="D44">
         <v>95.96</v>
       </c>
-      <c r="E44" t="s">
-        <v>17</v>
+      <c r="E44" t="b">
+        <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44">
         <v>2.16</v>
@@ -2945,19 +2996,19 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
         <v>101</v>
-      </c>
-      <c r="C45" t="s">
-        <v>102</v>
       </c>
       <c r="D45">
         <v>98</v>
       </c>
-      <c r="E45" t="s">
-        <v>17</v>
+      <c r="E45" t="b">
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G45">
         <v>1.9</v>
@@ -2980,19 +3031,19 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
         <v>103</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
       </c>
       <c r="D46">
         <v>101.07</v>
       </c>
-      <c r="E46" t="s">
-        <v>17</v>
+      <c r="E46" t="b">
+        <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G46">
         <v>2.2000000000000002</v>
@@ -3015,19 +3066,19 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" t="s">
         <v>105</v>
-      </c>
-      <c r="C47" t="s">
-        <v>106</v>
       </c>
       <c r="D47">
         <v>102.90600000000001</v>
       </c>
-      <c r="E47" t="s">
-        <v>17</v>
+      <c r="E47" t="b">
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G47">
         <v>2.2799999999999998</v>
@@ -3050,19 +3101,19 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
         <v>107</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
       </c>
       <c r="D48">
         <v>106.42</v>
       </c>
-      <c r="E48" t="s">
-        <v>17</v>
+      <c r="E48" t="b">
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G48">
         <v>2.2000000000000002</v>
@@ -3085,19 +3136,19 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" t="s">
         <v>109</v>
-      </c>
-      <c r="C49" t="s">
-        <v>110</v>
       </c>
       <c r="D49">
         <v>107.86799999999999</v>
       </c>
-      <c r="E49" t="s">
-        <v>17</v>
+      <c r="E49" t="b">
+        <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G49">
         <v>1.93</v>
@@ -3120,19 +3171,19 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
         <v>111</v>
-      </c>
-      <c r="C50" t="s">
-        <v>112</v>
       </c>
       <c r="D50">
         <v>112.411</v>
       </c>
-      <c r="E50" t="s">
-        <v>17</v>
+      <c r="E50" t="b">
+        <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G50">
         <v>1.69</v>
@@ -3155,16 +3206,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="s">
         <v>113</v>
-      </c>
-      <c r="C51" t="s">
-        <v>114</v>
       </c>
       <c r="D51">
         <v>114.818</v>
       </c>
-      <c r="E51" t="s">
-        <v>17</v>
+      <c r="E51" t="b">
+        <v>1</v>
       </c>
       <c r="F51" t="s">
         <v>4</v>
@@ -3190,16 +3241,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
         <v>115</v>
-      </c>
-      <c r="C52" t="s">
-        <v>116</v>
       </c>
       <c r="D52">
         <v>118.71</v>
       </c>
-      <c r="E52" t="s">
-        <v>17</v>
+      <c r="E52" t="b">
+        <v>1</v>
       </c>
       <c r="F52" t="s">
         <v>4</v>
@@ -3225,16 +3276,19 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" t="s">
         <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
       </c>
       <c r="D53">
         <v>121.76</v>
       </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
       <c r="F53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G53">
         <v>2.0499999999999998</v>
@@ -3257,16 +3311,19 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
         <v>119</v>
-      </c>
-      <c r="C54" t="s">
-        <v>120</v>
       </c>
       <c r="D54">
         <v>127.6</v>
       </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
       <c r="F54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G54">
         <v>2.1</v>
@@ -3289,16 +3346,19 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" t="s">
         <v>121</v>
-      </c>
-      <c r="C55" t="s">
-        <v>122</v>
       </c>
       <c r="D55">
         <v>126.904</v>
       </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
       <c r="F55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G55">
         <v>2.66</v>
@@ -3321,13 +3381,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
         <v>123</v>
-      </c>
-      <c r="C56" t="s">
-        <v>124</v>
       </c>
       <c r="D56">
         <v>131.29300000000001</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
       </c>
       <c r="F56" t="s">
         <v>14</v>
@@ -3350,19 +3413,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
         <v>125</v>
-      </c>
-      <c r="C57" t="s">
-        <v>126</v>
       </c>
       <c r="D57">
         <v>132.905</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
         <v>17</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
       </c>
       <c r="G57">
         <v>0.79</v>
@@ -3385,19 +3448,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" t="s">
         <v>127</v>
-      </c>
-      <c r="C58" t="s">
-        <v>128</v>
       </c>
       <c r="D58">
         <v>137.327</v>
       </c>
-      <c r="E58" t="s">
-        <v>17</v>
+      <c r="E58" t="b">
+        <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G58">
         <v>0.89</v>
@@ -3420,19 +3483,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
         <v>129</v>
-      </c>
-      <c r="C59" t="s">
-        <v>130</v>
       </c>
       <c r="D59">
         <v>138.905</v>
       </c>
-      <c r="E59" t="s">
-        <v>17</v>
+      <c r="E59" t="b">
+        <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G59">
         <v>1.1000000000000001</v>
@@ -3455,19 +3518,19 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60" t="s">
         <v>132</v>
-      </c>
-      <c r="C60" t="s">
-        <v>133</v>
       </c>
       <c r="D60">
         <v>140.11600000000001</v>
       </c>
-      <c r="E60" t="s">
-        <v>17</v>
+      <c r="E60" t="b">
+        <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G60">
         <v>1.1200000000000001</v>
@@ -3490,19 +3553,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" t="s">
         <v>134</v>
-      </c>
-      <c r="C61" t="s">
-        <v>135</v>
       </c>
       <c r="D61">
         <v>140.90799999999999</v>
       </c>
-      <c r="E61" t="s">
-        <v>17</v>
+      <c r="E61" t="b">
+        <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G61">
         <v>1.1299999999999999</v>
@@ -3525,19 +3588,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" t="s">
         <v>136</v>
-      </c>
-      <c r="C62" t="s">
-        <v>137</v>
       </c>
       <c r="D62">
         <v>144.24199999999999</v>
       </c>
-      <c r="E62" t="s">
-        <v>17</v>
+      <c r="E62" t="b">
+        <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G62">
         <v>1.1399999999999999</v>
@@ -3560,19 +3623,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" t="s">
         <v>138</v>
-      </c>
-      <c r="C63" t="s">
-        <v>139</v>
       </c>
       <c r="D63">
         <v>145</v>
       </c>
-      <c r="E63" t="s">
-        <v>17</v>
+      <c r="E63" t="b">
+        <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G63">
         <v>1.1299999999999999</v>
@@ -3595,19 +3658,19 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
         <v>140</v>
-      </c>
-      <c r="C64" t="s">
-        <v>141</v>
       </c>
       <c r="D64">
         <v>150.36000000000001</v>
       </c>
-      <c r="E64" t="s">
-        <v>17</v>
+      <c r="E64" t="b">
+        <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G64">
         <v>1.17</v>
@@ -3630,19 +3693,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" t="s">
         <v>142</v>
-      </c>
-      <c r="C65" t="s">
-        <v>143</v>
       </c>
       <c r="D65">
         <v>151.964</v>
       </c>
-      <c r="E65" t="s">
-        <v>17</v>
+      <c r="E65" t="b">
+        <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G65">
         <v>1.2</v>
@@ -3665,19 +3728,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" t="s">
         <v>144</v>
-      </c>
-      <c r="C66" t="s">
-        <v>145</v>
       </c>
       <c r="D66">
         <v>157.25</v>
       </c>
-      <c r="E66" t="s">
-        <v>17</v>
+      <c r="E66" t="b">
+        <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G66">
         <v>1.2</v>
@@ -3700,19 +3763,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" t="s">
         <v>146</v>
-      </c>
-      <c r="C67" t="s">
-        <v>147</v>
       </c>
       <c r="D67">
         <v>158.92500000000001</v>
       </c>
-      <c r="E67" t="s">
-        <v>17</v>
+      <c r="E67" t="b">
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G67">
         <v>1.2</v>
@@ -3735,19 +3798,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" t="s">
         <v>148</v>
-      </c>
-      <c r="C68" t="s">
-        <v>149</v>
       </c>
       <c r="D68">
         <v>162.5</v>
       </c>
-      <c r="E68" t="s">
-        <v>17</v>
+      <c r="E68" t="b">
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G68">
         <v>1.22</v>
@@ -3770,19 +3833,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" t="s">
         <v>150</v>
-      </c>
-      <c r="C69" t="s">
-        <v>151</v>
       </c>
       <c r="D69">
         <v>164.93</v>
       </c>
-      <c r="E69" t="s">
-        <v>17</v>
+      <c r="E69" t="b">
+        <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G69">
         <v>1.23</v>
@@ -3805,19 +3868,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" t="s">
         <v>152</v>
-      </c>
-      <c r="C70" t="s">
-        <v>153</v>
       </c>
       <c r="D70">
         <v>167.25899999999999</v>
       </c>
-      <c r="E70" t="s">
-        <v>17</v>
+      <c r="E70" t="b">
+        <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G70">
         <v>1.24</v>
@@ -3840,19 +3903,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" t="s">
         <v>154</v>
-      </c>
-      <c r="C71" t="s">
-        <v>155</v>
       </c>
       <c r="D71">
         <v>168.934</v>
       </c>
-      <c r="E71" t="s">
-        <v>17</v>
+      <c r="E71" t="b">
+        <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G71">
         <v>1.25</v>
@@ -3875,19 +3938,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" t="s">
         <v>156</v>
-      </c>
-      <c r="C72" t="s">
-        <v>157</v>
       </c>
       <c r="D72">
         <v>173.054</v>
       </c>
-      <c r="E72" t="s">
-        <v>17</v>
+      <c r="E72" t="b">
+        <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G72">
         <v>1.1000000000000001</v>
@@ -3910,19 +3973,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" t="s">
         <v>158</v>
-      </c>
-      <c r="C73" t="s">
-        <v>159</v>
       </c>
       <c r="D73">
         <v>174.96700000000001</v>
       </c>
-      <c r="E73" t="s">
-        <v>17</v>
+      <c r="E73" t="b">
+        <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G73">
         <v>1.27</v>
@@ -3945,19 +4008,19 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>159</v>
+      </c>
+      <c r="C74" t="s">
         <v>160</v>
-      </c>
-      <c r="C74" t="s">
-        <v>161</v>
       </c>
       <c r="D74">
         <v>178.49</v>
       </c>
-      <c r="E74" t="s">
-        <v>17</v>
+      <c r="E74" t="b">
+        <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G74">
         <v>1.3</v>
@@ -3980,19 +4043,19 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>161</v>
+      </c>
+      <c r="C75" t="s">
         <v>162</v>
-      </c>
-      <c r="C75" t="s">
-        <v>163</v>
       </c>
       <c r="D75">
         <v>180.94800000000001</v>
       </c>
-      <c r="E75" t="s">
-        <v>17</v>
+      <c r="E75" t="b">
+        <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G75">
         <v>1.5</v>
@@ -4015,19 +4078,19 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" t="s">
         <v>164</v>
-      </c>
-      <c r="C76" t="s">
-        <v>165</v>
       </c>
       <c r="D76">
         <v>183.84</v>
       </c>
-      <c r="E76" t="s">
-        <v>17</v>
+      <c r="E76" t="b">
+        <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G76">
         <v>2.36</v>
@@ -4050,19 +4113,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" t="s">
         <v>166</v>
-      </c>
-      <c r="C77" t="s">
-        <v>167</v>
       </c>
       <c r="D77">
         <v>186.20699999999999</v>
       </c>
-      <c r="E77" t="s">
-        <v>17</v>
+      <c r="E77" t="b">
+        <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G77">
         <v>1.9</v>
@@ -4085,19 +4148,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" t="s">
         <v>168</v>
-      </c>
-      <c r="C78" t="s">
-        <v>169</v>
       </c>
       <c r="D78">
         <v>190.23</v>
       </c>
-      <c r="E78" t="s">
-        <v>17</v>
+      <c r="E78" t="b">
+        <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G78">
         <v>2.2000000000000002</v>
@@ -4120,19 +4183,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" t="s">
         <v>170</v>
-      </c>
-      <c r="C79" t="s">
-        <v>171</v>
       </c>
       <c r="D79">
         <v>192.21700000000001</v>
       </c>
-      <c r="E79" t="s">
-        <v>17</v>
+      <c r="E79" t="b">
+        <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G79">
         <v>2.2000000000000002</v>
@@ -4155,19 +4218,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
         <v>172</v>
-      </c>
-      <c r="C80" t="s">
-        <v>173</v>
       </c>
       <c r="D80">
         <v>195.084</v>
       </c>
-      <c r="E80" t="s">
-        <v>17</v>
+      <c r="E80" t="b">
+        <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G80">
         <v>2.2799999999999998</v>
@@ -4190,19 +4253,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" t="s">
         <v>174</v>
-      </c>
-      <c r="C81" t="s">
-        <v>175</v>
       </c>
       <c r="D81">
         <v>196.96700000000001</v>
       </c>
-      <c r="E81" t="s">
-        <v>17</v>
+      <c r="E81" t="b">
+        <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G81">
         <v>2.54</v>
@@ -4225,19 +4288,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" t="s">
         <v>176</v>
-      </c>
-      <c r="C82" t="s">
-        <v>177</v>
       </c>
       <c r="D82">
         <v>200.59</v>
       </c>
-      <c r="E82" t="s">
-        <v>17</v>
+      <c r="E82" t="b">
+        <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G82">
         <v>2</v>
@@ -4260,16 +4323,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" t="s">
         <v>178</v>
-      </c>
-      <c r="C83" t="s">
-        <v>179</v>
       </c>
       <c r="D83">
         <v>204.38300000000001</v>
       </c>
-      <c r="E83" t="s">
-        <v>17</v>
+      <c r="E83" t="b">
+        <v>1</v>
       </c>
       <c r="F83" t="s">
         <v>4</v>
@@ -4295,16 +4358,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" t="s">
         <v>180</v>
-      </c>
-      <c r="C84" t="s">
-        <v>181</v>
       </c>
       <c r="D84">
         <v>207.2</v>
       </c>
-      <c r="E84" t="s">
-        <v>17</v>
+      <c r="E84" t="b">
+        <v>1</v>
       </c>
       <c r="F84" t="s">
         <v>4</v>
@@ -4330,16 +4393,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>181</v>
+      </c>
+      <c r="C85" t="s">
         <v>182</v>
-      </c>
-      <c r="C85" t="s">
-        <v>183</v>
       </c>
       <c r="D85">
         <v>208.98</v>
       </c>
-      <c r="E85" t="s">
-        <v>17</v>
+      <c r="E85" t="b">
+        <v>1</v>
       </c>
       <c r="F85" t="s">
         <v>4</v>
@@ -4365,16 +4428,19 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" t="s">
         <v>184</v>
-      </c>
-      <c r="C86" t="s">
-        <v>185</v>
       </c>
       <c r="D86">
         <v>210</v>
       </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
       <c r="F86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G86">
         <v>2</v>
@@ -4397,13 +4463,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" t="s">
         <v>186</v>
-      </c>
-      <c r="C87" t="s">
-        <v>187</v>
       </c>
       <c r="D87">
         <v>210</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
       </c>
       <c r="F87" t="s">
         <v>14</v>
@@ -4429,19 +4498,19 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" t="s">
         <v>188</v>
-      </c>
-      <c r="C88" t="s">
-        <v>189</v>
       </c>
       <c r="D88">
         <v>222</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
         <v>17</v>
-      </c>
-      <c r="F88" t="s">
-        <v>18</v>
       </c>
       <c r="H88">
         <v>10.7485</v>
@@ -4461,19 +4530,19 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" t="s">
         <v>190</v>
-      </c>
-      <c r="C89" t="s">
-        <v>191</v>
       </c>
       <c r="D89">
         <v>223</v>
       </c>
-      <c r="E89" t="s">
-        <v>17</v>
+      <c r="E89" t="b">
+        <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G89">
         <v>0.7</v>
@@ -4496,19 +4565,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" t="s">
         <v>192</v>
-      </c>
-      <c r="C90" t="s">
-        <v>193</v>
       </c>
       <c r="D90">
         <v>226</v>
       </c>
-      <c r="E90" t="s">
-        <v>17</v>
+      <c r="E90" t="b">
+        <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G90">
         <v>0.9</v>
@@ -4531,19 +4600,19 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
+        <v>194</v>
+      </c>
+      <c r="C91" t="s">
         <v>195</v>
-      </c>
-      <c r="C91" t="s">
-        <v>196</v>
       </c>
       <c r="D91">
         <v>227</v>
       </c>
-      <c r="E91" t="s">
-        <v>17</v>
+      <c r="E91" t="b">
+        <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G91">
         <v>1.1000000000000001</v>
@@ -4566,19 +4635,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" t="s">
         <v>197</v>
-      </c>
-      <c r="C92" t="s">
-        <v>198</v>
       </c>
       <c r="D92">
         <v>232.03800000000001</v>
       </c>
-      <c r="E92" t="s">
-        <v>17</v>
+      <c r="E92" t="b">
+        <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G92">
         <v>1.3</v>
@@ -4601,19 +4670,19 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" t="s">
         <v>199</v>
-      </c>
-      <c r="C93" t="s">
-        <v>200</v>
       </c>
       <c r="D93">
         <v>231.036</v>
       </c>
-      <c r="E93" t="s">
-        <v>17</v>
+      <c r="E93" t="b">
+        <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G93">
         <v>1.5</v>
@@ -4636,19 +4705,19 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
+        <v>200</v>
+      </c>
+      <c r="C94" t="s">
         <v>201</v>
-      </c>
-      <c r="C94" t="s">
-        <v>202</v>
       </c>
       <c r="D94">
         <v>238.029</v>
       </c>
-      <c r="E94" t="s">
-        <v>17</v>
+      <c r="E94" t="b">
+        <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G94">
         <v>1.38</v>
@@ -4671,19 +4740,19 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
+        <v>202</v>
+      </c>
+      <c r="C95" t="s">
         <v>203</v>
-      </c>
-      <c r="C95" t="s">
-        <v>204</v>
       </c>
       <c r="D95">
         <v>237</v>
       </c>
-      <c r="E95" t="s">
-        <v>17</v>
+      <c r="E95" t="b">
+        <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G95">
         <v>1.36</v>
@@ -4706,19 +4775,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
+        <v>204</v>
+      </c>
+      <c r="C96" t="s">
         <v>205</v>
-      </c>
-      <c r="C96" t="s">
-        <v>206</v>
       </c>
       <c r="D96">
         <v>244</v>
       </c>
-      <c r="E96" t="s">
-        <v>17</v>
+      <c r="E96" t="b">
+        <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G96">
         <v>1.28</v>
@@ -4741,19 +4810,19 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>206</v>
+      </c>
+      <c r="C97" t="s">
         <v>207</v>
-      </c>
-      <c r="C97" t="s">
-        <v>208</v>
       </c>
       <c r="D97">
         <v>243</v>
       </c>
-      <c r="E97" t="s">
-        <v>17</v>
+      <c r="E97" t="b">
+        <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G97">
         <v>1.3</v>
@@ -4776,19 +4845,19 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>208</v>
+      </c>
+      <c r="C98" t="s">
         <v>209</v>
-      </c>
-      <c r="C98" t="s">
-        <v>210</v>
       </c>
       <c r="D98">
         <v>247</v>
       </c>
-      <c r="E98" t="s">
-        <v>17</v>
+      <c r="E98" t="b">
+        <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G98">
         <v>1.3</v>
@@ -4811,19 +4880,19 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" t="s">
         <v>211</v>
-      </c>
-      <c r="C99" t="s">
-        <v>212</v>
       </c>
       <c r="D99">
         <v>247</v>
       </c>
-      <c r="E99" t="s">
-        <v>17</v>
+      <c r="E99" t="b">
+        <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G99">
         <v>1.3</v>
@@ -4846,19 +4915,19 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>212</v>
+      </c>
+      <c r="C100" t="s">
         <v>213</v>
-      </c>
-      <c r="C100" t="s">
-        <v>214</v>
       </c>
       <c r="D100">
         <v>251</v>
       </c>
-      <c r="E100" t="s">
-        <v>17</v>
+      <c r="E100" t="b">
+        <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G100">
         <v>1.3</v>
@@ -4881,19 +4950,19 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>214</v>
+      </c>
+      <c r="C101" t="s">
         <v>215</v>
-      </c>
-      <c r="C101" t="s">
-        <v>216</v>
       </c>
       <c r="D101">
         <v>252</v>
       </c>
-      <c r="E101" t="s">
-        <v>17</v>
+      <c r="E101" t="b">
+        <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G101">
         <v>1.3</v>
@@ -4913,19 +4982,19 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
+        <v>216</v>
+      </c>
+      <c r="C102" t="s">
         <v>217</v>
-      </c>
-      <c r="C102" t="s">
-        <v>218</v>
       </c>
       <c r="D102">
         <v>257</v>
       </c>
-      <c r="E102" t="s">
-        <v>17</v>
+      <c r="E102" t="b">
+        <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G102">
         <v>1.3</v>
@@ -4939,19 +5008,19 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
+        <v>218</v>
+      </c>
+      <c r="C103" t="s">
         <v>219</v>
-      </c>
-      <c r="C103" t="s">
-        <v>220</v>
       </c>
       <c r="D103">
         <v>258</v>
       </c>
-      <c r="E103" t="s">
-        <v>17</v>
+      <c r="E103" t="b">
+        <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G103">
         <v>1.3</v>
@@ -4965,19 +5034,19 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
+        <v>220</v>
+      </c>
+      <c r="C104" t="s">
         <v>221</v>
-      </c>
-      <c r="C104" t="s">
-        <v>222</v>
       </c>
       <c r="D104">
         <v>259</v>
       </c>
-      <c r="E104" t="s">
-        <v>17</v>
+      <c r="E104" t="b">
+        <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G104">
         <v>1.3</v>
@@ -4991,19 +5060,19 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
+        <v>222</v>
+      </c>
+      <c r="C105" t="s">
         <v>223</v>
-      </c>
-      <c r="C105" t="s">
-        <v>224</v>
       </c>
       <c r="D105">
         <v>262</v>
       </c>
-      <c r="E105" t="s">
-        <v>17</v>
+      <c r="E105" t="b">
+        <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -5011,19 +5080,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
+        <v>224</v>
+      </c>
+      <c r="C106" t="s">
         <v>225</v>
-      </c>
-      <c r="C106" t="s">
-        <v>226</v>
       </c>
       <c r="D106">
         <v>261</v>
       </c>
-      <c r="E106" t="s">
-        <v>17</v>
+      <c r="E106" t="b">
+        <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I106" s="1">
         <v>18.100000000000001</v>
@@ -5034,19 +5103,19 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
+        <v>227</v>
+      </c>
+      <c r="C107" t="s">
         <v>228</v>
-      </c>
-      <c r="C107" t="s">
-        <v>229</v>
       </c>
       <c r="D107">
         <v>262</v>
       </c>
-      <c r="E107" t="s">
-        <v>17</v>
+      <c r="E107" t="b">
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I107" s="1">
         <v>39</v>
@@ -5057,19 +5126,19 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
+        <v>229</v>
+      </c>
+      <c r="C108" t="s">
         <v>230</v>
-      </c>
-      <c r="C108" t="s">
-        <v>231</v>
       </c>
       <c r="D108">
         <v>266</v>
       </c>
-      <c r="E108" t="s">
-        <v>17</v>
+      <c r="E108" t="b">
+        <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I108" s="1">
         <v>35</v>
@@ -5080,19 +5149,19 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
+        <v>231</v>
+      </c>
+      <c r="C109" t="s">
         <v>232</v>
-      </c>
-      <c r="C109" t="s">
-        <v>233</v>
       </c>
       <c r="D109">
         <v>264</v>
       </c>
-      <c r="E109" t="s">
-        <v>17</v>
+      <c r="E109" t="b">
+        <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I109" s="1">
         <v>37</v>
@@ -5103,19 +5172,19 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
+        <v>233</v>
+      </c>
+      <c r="C110" t="s">
         <v>234</v>
-      </c>
-      <c r="C110" t="s">
-        <v>235</v>
       </c>
       <c r="D110">
         <v>267</v>
       </c>
-      <c r="E110" t="s">
-        <v>17</v>
+      <c r="E110" t="b">
+        <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I110" s="1">
         <v>41</v>
@@ -5126,19 +5195,19 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
+        <v>235</v>
+      </c>
+      <c r="C111" t="s">
         <v>236</v>
-      </c>
-      <c r="C111" t="s">
-        <v>237</v>
       </c>
       <c r="D111">
         <v>268</v>
       </c>
-      <c r="E111" t="s">
-        <v>17</v>
+      <c r="E111" t="b">
+        <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I111" s="1">
         <v>35</v>
@@ -5149,19 +5218,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
+        <v>237</v>
+      </c>
+      <c r="C112" t="s">
         <v>238</v>
-      </c>
-      <c r="C112" t="s">
-        <v>239</v>
       </c>
       <c r="D112">
         <v>271</v>
       </c>
-      <c r="E112" t="s">
-        <v>17</v>
+      <c r="E112" t="b">
+        <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -5169,19 +5238,19 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
+        <v>239</v>
+      </c>
+      <c r="C113" t="s">
         <v>240</v>
-      </c>
-      <c r="C113" t="s">
-        <v>241</v>
       </c>
       <c r="D113">
         <v>272</v>
       </c>
-      <c r="E113" t="s">
-        <v>17</v>
+      <c r="E113" t="b">
+        <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -5189,19 +5258,19 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
+        <v>241</v>
+      </c>
+      <c r="C114" t="s">
         <v>242</v>
-      </c>
-      <c r="C114" t="s">
-        <v>243</v>
       </c>
       <c r="D114">
         <v>285</v>
       </c>
-      <c r="E114" t="s">
-        <v>17</v>
+      <c r="E114" t="b">
+        <v>1</v>
       </c>
       <c r="F114" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -5209,16 +5278,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
+        <v>243</v>
+      </c>
+      <c r="C115" t="s">
         <v>244</v>
-      </c>
-      <c r="C115" t="s">
-        <v>245</v>
       </c>
       <c r="D115">
         <v>284</v>
       </c>
-      <c r="E115" t="s">
-        <v>17</v>
+      <c r="E115" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -5226,19 +5295,19 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
+        <v>245</v>
+      </c>
+      <c r="C116" t="s">
         <v>246</v>
-      </c>
-      <c r="C116" t="s">
-        <v>247</v>
       </c>
       <c r="D116">
         <v>289</v>
       </c>
-      <c r="E116" t="s">
-        <v>17</v>
+      <c r="E116" t="b">
+        <v>1</v>
       </c>
       <c r="F116" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -5246,16 +5315,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
+        <v>247</v>
+      </c>
+      <c r="C117" t="s">
         <v>248</v>
-      </c>
-      <c r="C117" t="s">
-        <v>249</v>
       </c>
       <c r="D117">
         <v>288</v>
       </c>
-      <c r="E117" t="s">
-        <v>17</v>
+      <c r="E117" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -5263,19 +5332,19 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
+        <v>249</v>
+      </c>
+      <c r="C118" t="s">
         <v>250</v>
-      </c>
-      <c r="C118" t="s">
-        <v>251</v>
       </c>
       <c r="D118">
         <v>292</v>
       </c>
-      <c r="E118" t="s">
-        <v>17</v>
+      <c r="E118" t="b">
+        <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -5283,13 +5352,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
+        <v>251</v>
+      </c>
+      <c r="C119" t="s">
         <v>252</v>
-      </c>
-      <c r="C119" t="s">
-        <v>253</v>
       </c>
       <c r="D119">
         <v>295</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -5297,13 +5369,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
+        <v>253</v>
+      </c>
+      <c r="C120" t="s">
         <v>254</v>
-      </c>
-      <c r="C120" t="s">
-        <v>255</v>
       </c>
       <c r="D120">
         <v>294</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
       </c>
       <c r="F120" t="s">
         <v>14</v>
@@ -5336,79 +5411,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
         <v>267</v>
-      </c>
-      <c r="B1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" t="s">
         <v>280</v>
-      </c>
-      <c r="B5" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" t="s">
         <v>282</v>
-      </c>
-      <c r="B6" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" t="s">
         <v>284</v>
-      </c>
-      <c r="B7" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" t="s">
         <v>290</v>
-      </c>
-      <c r="B9" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" t="s">
         <v>293</v>
-      </c>
-      <c r="B10" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TryParse to all generated enums in the rococo.carpenter application. We still need to do some testing. We also need to add optional reverse lookup tables.
</commit_message>
<xml_diff>
--- a/tables/periodic-table.xlsx
+++ b/tables/periodic-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD4F0AC-2668-437C-A450-7A08601455A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4119549D-2003-45B9-AA44-7BE7030AD590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="303">
   <si>
     <t>AtomicNumber</t>
   </si>
@@ -942,6 +942,9 @@
   </si>
   <si>
     <t>Int32</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3230684E-8A11-41FB-8526-9EA18FC7052C}">
-  <dimension ref="A1:K120"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,220 +1541,220 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>302</v>
       </c>
       <c r="D3">
-        <v>1.0069999999999999</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>302</v>
       </c>
       <c r="G3">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>13.5984</v>
-      </c>
-      <c r="I3" s="1">
-        <v>8.9900000000000003E-5</v>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>14.175000000000001</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>20.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>4.0019999999999998</v>
+        <v>1.0069999999999999</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>2.2000000000000002</v>
       </c>
       <c r="H4">
-        <v>24.587399999999999</v>
+        <v>13.5984</v>
       </c>
       <c r="I4" s="1">
-        <v>1.7899999999999999E-4</v>
+        <v>8.9900000000000003E-5</v>
+      </c>
+      <c r="J4">
+        <v>14.175000000000001</v>
       </c>
       <c r="K4">
-        <v>4.22</v>
+        <v>20.28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>6.9409999999999998</v>
+        <v>4.0019999999999998</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>0.98</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>5.3917000000000002</v>
+        <v>24.587399999999999</v>
       </c>
       <c r="I5" s="1">
-        <v>0.53400000000000003</v>
-      </c>
-      <c r="J5">
-        <v>453.85</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="K5">
-        <v>1615</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>9.0120000000000005</v>
+        <v>6.9409999999999998</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G6">
-        <v>1.57</v>
+        <v>0.98</v>
       </c>
       <c r="H6">
-        <v>9.3226999999999993</v>
+        <v>5.3917000000000002</v>
       </c>
       <c r="I6" s="1">
-        <v>1.85</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="J6">
-        <v>1560.15</v>
+        <v>453.85</v>
       </c>
       <c r="K6">
-        <v>2742</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>10.811</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>2.04</v>
+        <v>1.57</v>
       </c>
       <c r="H7">
-        <v>8.298</v>
+        <v>9.3226999999999993</v>
       </c>
       <c r="I7" s="1">
-        <v>2.34</v>
+        <v>1.85</v>
       </c>
       <c r="J7">
-        <v>2573.15</v>
+        <v>1560.15</v>
       </c>
       <c r="K7">
-        <v>4200</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>12.010999999999999</v>
+        <v>10.811</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G8">
-        <v>2.5499999999999998</v>
+        <v>2.04</v>
       </c>
       <c r="H8">
-        <v>11.260300000000001</v>
+        <v>8.298</v>
       </c>
       <c r="I8" s="1">
-        <v>2.27</v>
+        <v>2.34</v>
       </c>
       <c r="J8">
-        <v>3948.15</v>
+        <v>2573.15</v>
       </c>
       <c r="K8">
-        <v>4300</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>14.007</v>
+        <v>12.010999999999999</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1760,33 +1763,33 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>3.04</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="H9">
-        <v>14.5341</v>
+        <v>11.260300000000001</v>
       </c>
       <c r="I9" s="1">
-        <v>1.25E-3</v>
+        <v>2.27</v>
       </c>
       <c r="J9">
-        <v>63.29</v>
+        <v>3948.15</v>
       </c>
       <c r="K9">
-        <v>77.36</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>15.999000000000001</v>
+        <v>14.007</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1795,275 +1798,275 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>3.44</v>
+        <v>3.04</v>
       </c>
       <c r="H10">
-        <v>13.6181</v>
+        <v>14.5341</v>
       </c>
       <c r="I10" s="1">
-        <v>1.4300000000000001E-3</v>
+        <v>1.25E-3</v>
       </c>
       <c r="J10">
-        <v>50.5</v>
+        <v>63.29</v>
       </c>
       <c r="K10">
-        <v>90.2</v>
+        <v>77.36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>18.998000000000001</v>
+        <v>15.999000000000001</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>3.98</v>
+        <v>3.44</v>
       </c>
       <c r="H11">
-        <v>17.422799999999999</v>
+        <v>13.6181</v>
       </c>
       <c r="I11" s="1">
-        <v>1.6999999999999999E-3</v>
+        <v>1.4300000000000001E-3</v>
       </c>
       <c r="J11">
-        <v>53.63</v>
+        <v>50.5</v>
       </c>
       <c r="K11">
-        <v>85.03</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12">
-        <v>20.18</v>
+        <v>18.998000000000001</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>3.98</v>
       </c>
       <c r="H12">
-        <v>21.564499999999999</v>
+        <v>17.422799999999999</v>
       </c>
       <c r="I12" s="1">
-        <v>8.9999999999999998E-4</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="J12">
-        <v>24.702999999999999</v>
+        <v>53.63</v>
       </c>
       <c r="K12">
-        <v>27.07</v>
+        <v>85.03</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>22.99</v>
+        <v>20.18</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>0.93</v>
+        <v>14</v>
       </c>
       <c r="H13">
-        <v>5.1391</v>
+        <v>21.564499999999999</v>
       </c>
       <c r="I13" s="1">
-        <v>0.97099999999999997</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="J13">
-        <v>371.15</v>
+        <v>24.702999999999999</v>
       </c>
       <c r="K13">
-        <v>1156</v>
+        <v>27.07</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>24.305</v>
+        <v>22.99</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G14">
-        <v>1.31</v>
+        <v>0.93</v>
       </c>
       <c r="H14">
-        <v>7.6462000000000003</v>
+        <v>5.1391</v>
       </c>
       <c r="I14" s="1">
-        <v>1.74</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="J14">
-        <v>923.15</v>
+        <v>371.15</v>
       </c>
       <c r="K14">
-        <v>1363</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15">
-        <v>26.981999999999999</v>
+        <v>24.305</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G15">
-        <v>1.61</v>
+        <v>1.31</v>
       </c>
       <c r="H15">
-        <v>5.9858000000000002</v>
+        <v>7.6462000000000003</v>
       </c>
       <c r="I15" s="1">
-        <v>2.7</v>
+        <v>1.74</v>
       </c>
       <c r="J15">
-        <v>933.4</v>
+        <v>923.15</v>
       </c>
       <c r="K15">
-        <v>2792</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>28.085999999999999</v>
+        <v>26.981999999999999</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>1.9</v>
+        <v>1.61</v>
       </c>
       <c r="H16">
-        <v>8.1516999999999999</v>
+        <v>5.9858000000000002</v>
       </c>
       <c r="I16" s="1">
-        <v>2.33</v>
+        <v>2.7</v>
       </c>
       <c r="J16">
-        <v>1683.15</v>
+        <v>933.4</v>
       </c>
       <c r="K16">
-        <v>3538</v>
+        <v>2792</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17">
-        <v>30.974</v>
+        <v>28.085999999999999</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G17">
-        <v>2.19</v>
+        <v>1.9</v>
       </c>
       <c r="H17">
-        <v>10.486700000000001</v>
+        <v>8.1516999999999999</v>
       </c>
       <c r="I17" s="1">
-        <v>1.82</v>
+        <v>2.33</v>
       </c>
       <c r="J17">
-        <v>317.25</v>
+        <v>1683.15</v>
       </c>
       <c r="K17">
-        <v>553</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18">
-        <v>32.064999999999998</v>
+        <v>30.974</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -2072,205 +2075,205 @@
         <v>11</v>
       </c>
       <c r="G18">
-        <v>2.58</v>
+        <v>2.19</v>
       </c>
       <c r="H18">
-        <v>10.36</v>
+        <v>10.486700000000001</v>
       </c>
       <c r="I18" s="1">
-        <v>2.0699999999999998</v>
+        <v>1.82</v>
       </c>
       <c r="J18">
-        <v>388.51</v>
+        <v>317.25</v>
       </c>
       <c r="K18">
-        <v>717.8</v>
+        <v>553</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19">
-        <v>35.453000000000003</v>
+        <v>32.064999999999998</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>3.16</v>
+        <v>2.58</v>
       </c>
       <c r="H19">
-        <v>12.967599999999999</v>
+        <v>10.36</v>
       </c>
       <c r="I19" s="1">
-        <v>3.2100000000000002E-3</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="J19">
-        <v>172.31</v>
+        <v>388.51</v>
       </c>
       <c r="K19">
-        <v>239.11</v>
+        <v>717.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D20">
-        <v>39.948</v>
+        <v>35.453000000000003</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="G20">
+        <v>3.16</v>
       </c>
       <c r="H20">
-        <v>15.759600000000001</v>
+        <v>12.967599999999999</v>
       </c>
       <c r="I20" s="1">
-        <v>1.7799999999999999E-3</v>
+        <v>3.2100000000000002E-3</v>
       </c>
       <c r="J20">
-        <v>83.96</v>
+        <v>172.31</v>
       </c>
       <c r="K20">
-        <v>87.3</v>
+        <v>239.11</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>39.097999999999999</v>
+        <v>39.948</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21">
-        <v>0.82</v>
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>4.3407</v>
+        <v>15.759600000000001</v>
       </c>
       <c r="I21" s="1">
-        <v>0.86199999999999999</v>
+        <v>1.7799999999999999E-3</v>
       </c>
       <c r="J21">
-        <v>336.5</v>
+        <v>83.96</v>
       </c>
       <c r="K21">
-        <v>1032</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>40.078000000000003</v>
+        <v>39.097999999999999</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="H22">
-        <v>6.1132</v>
+        <v>4.3407</v>
       </c>
       <c r="I22" s="1">
-        <v>1.54</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="J22">
-        <v>1112.1500000000001</v>
+        <v>336.5</v>
       </c>
       <c r="K22">
-        <v>1757</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23">
-        <v>44.956000000000003</v>
+        <v>40.078000000000003</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="G23">
-        <v>1.36</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>6.5614999999999997</v>
+        <v>6.1132</v>
       </c>
       <c r="I23" s="1">
-        <v>2.99</v>
+        <v>1.54</v>
       </c>
       <c r="J23">
-        <v>1812.15</v>
+        <v>1112.1500000000001</v>
       </c>
       <c r="K23">
-        <v>3109</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24">
-        <v>47.866999999999997</v>
+        <v>44.956000000000003</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -2279,33 +2282,33 @@
         <v>57</v>
       </c>
       <c r="G24">
-        <v>1.54</v>
+        <v>1.36</v>
       </c>
       <c r="H24">
-        <v>6.8281000000000001</v>
+        <v>6.5614999999999997</v>
       </c>
       <c r="I24" s="1">
-        <v>4.54</v>
+        <v>2.99</v>
       </c>
       <c r="J24">
-        <v>1933.15</v>
+        <v>1812.15</v>
       </c>
       <c r="K24">
-        <v>3560</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25">
-        <v>50.942</v>
+        <v>47.866999999999997</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -2314,33 +2317,33 @@
         <v>57</v>
       </c>
       <c r="G25">
-        <v>1.63</v>
+        <v>1.54</v>
       </c>
       <c r="H25">
-        <v>6.7462</v>
+        <v>6.8281000000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>6.11</v>
+        <v>4.54</v>
       </c>
       <c r="J25">
-        <v>2175.15</v>
+        <v>1933.15</v>
       </c>
       <c r="K25">
-        <v>3680</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26">
-        <v>51.996000000000002</v>
+        <v>50.942</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -2349,33 +2352,33 @@
         <v>57</v>
       </c>
       <c r="G26">
-        <v>1.66</v>
+        <v>1.63</v>
       </c>
       <c r="H26">
-        <v>6.7664999999999997</v>
+        <v>6.7462</v>
       </c>
       <c r="I26" s="1">
-        <v>7.15</v>
+        <v>6.11</v>
       </c>
       <c r="J26">
-        <v>2130.15</v>
+        <v>2175.15</v>
       </c>
       <c r="K26">
-        <v>2944</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27">
-        <v>54.938000000000002</v>
+        <v>51.996000000000002</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -2384,33 +2387,33 @@
         <v>57</v>
       </c>
       <c r="G27">
-        <v>1.55</v>
+        <v>1.66</v>
       </c>
       <c r="H27">
-        <v>7.4340000000000002</v>
+        <v>6.7664999999999997</v>
       </c>
       <c r="I27" s="1">
-        <v>7.44</v>
+        <v>7.15</v>
       </c>
       <c r="J27">
-        <v>1519.15</v>
+        <v>2130.15</v>
       </c>
       <c r="K27">
-        <v>2334</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28">
-        <v>55.844999999999999</v>
+        <v>54.938000000000002</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -2419,33 +2422,33 @@
         <v>57</v>
       </c>
       <c r="G28">
-        <v>1.83</v>
+        <v>1.55</v>
       </c>
       <c r="H28">
-        <v>7.9024000000000001</v>
+        <v>7.4340000000000002</v>
       </c>
       <c r="I28" s="1">
-        <v>7.87</v>
+        <v>7.44</v>
       </c>
       <c r="J28">
-        <v>1808.15</v>
+        <v>1519.15</v>
       </c>
       <c r="K28">
-        <v>3134</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D29">
-        <v>58.933</v>
+        <v>55.844999999999999</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -2454,33 +2457,33 @@
         <v>57</v>
       </c>
       <c r="G29">
-        <v>1.88</v>
+        <v>1.83</v>
       </c>
       <c r="H29">
-        <v>7.8810000000000002</v>
+        <v>7.9024000000000001</v>
       </c>
       <c r="I29" s="1">
-        <v>8.86</v>
+        <v>7.87</v>
       </c>
       <c r="J29">
-        <v>1768.15</v>
+        <v>1808.15</v>
       </c>
       <c r="K29">
-        <v>3200</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D30">
-        <v>58.692999999999998</v>
+        <v>58.933</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -2489,33 +2492,33 @@
         <v>57</v>
       </c>
       <c r="G30">
-        <v>1.91</v>
+        <v>1.88</v>
       </c>
       <c r="H30">
-        <v>7.6398000000000001</v>
+        <v>7.8810000000000002</v>
       </c>
       <c r="I30" s="1">
-        <v>8.91</v>
+        <v>8.86</v>
       </c>
       <c r="J30">
-        <v>1726.15</v>
+        <v>1768.15</v>
       </c>
       <c r="K30">
-        <v>3186</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D31">
-        <v>63.545999999999999</v>
+        <v>58.692999999999998</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -2524,33 +2527,33 @@
         <v>57</v>
       </c>
       <c r="G31">
-        <v>1.9</v>
+        <v>1.91</v>
       </c>
       <c r="H31">
-        <v>7.7263999999999999</v>
+        <v>7.6398000000000001</v>
       </c>
       <c r="I31" s="1">
-        <v>8.9600000000000009</v>
+        <v>8.91</v>
       </c>
       <c r="J31">
-        <v>1357.75</v>
+        <v>1726.15</v>
       </c>
       <c r="K31">
-        <v>2835</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D32">
-        <v>65.38</v>
+        <v>63.545999999999999</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -2559,103 +2562,103 @@
         <v>57</v>
       </c>
       <c r="G32">
-        <v>1.65</v>
+        <v>1.9</v>
       </c>
       <c r="H32">
-        <v>9.3941999999999997</v>
+        <v>7.7263999999999999</v>
       </c>
       <c r="I32" s="1">
-        <v>7.13</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="J32">
-        <v>692.88</v>
+        <v>1357.75</v>
       </c>
       <c r="K32">
-        <v>1180</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D33">
-        <v>69.722999999999999</v>
+        <v>65.38</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G33">
-        <v>1.81</v>
+        <v>1.65</v>
       </c>
       <c r="H33">
-        <v>5.9992999999999999</v>
+        <v>9.3941999999999997</v>
       </c>
       <c r="I33" s="1">
-        <v>5.91</v>
+        <v>7.13</v>
       </c>
       <c r="J33">
-        <v>302.91000000000003</v>
+        <v>692.88</v>
       </c>
       <c r="K33">
-        <v>2477</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34">
-        <v>72.64</v>
+        <v>69.722999999999999</v>
       </c>
       <c r="E34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G34">
-        <v>2.0099999999999998</v>
+        <v>1.81</v>
       </c>
       <c r="H34">
-        <v>7.8994</v>
+        <v>5.9992999999999999</v>
       </c>
       <c r="I34" s="1">
-        <v>5.32</v>
+        <v>5.91</v>
       </c>
       <c r="J34">
-        <v>1211.45</v>
+        <v>302.91000000000003</v>
       </c>
       <c r="K34">
-        <v>3106</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D35">
-        <v>74.921999999999997</v>
+        <v>72.64</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -2664,240 +2667,240 @@
         <v>23</v>
       </c>
       <c r="G35">
-        <v>2.1800000000000002</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="H35">
-        <v>9.7886000000000006</v>
+        <v>7.8994</v>
       </c>
       <c r="I35" s="1">
-        <v>5.78</v>
+        <v>5.32</v>
       </c>
       <c r="J35">
-        <v>1090.1500000000001</v>
+        <v>1211.45</v>
       </c>
       <c r="K35">
-        <v>887</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36">
-        <v>78.959999999999994</v>
+        <v>74.921999999999997</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G36">
-        <v>2.5499999999999998</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="H36">
-        <v>9.7523999999999997</v>
+        <v>9.7886000000000006</v>
       </c>
       <c r="I36" s="1">
-        <v>4.8099999999999996</v>
+        <v>5.78</v>
       </c>
       <c r="J36">
-        <v>494.15</v>
+        <v>1090.1500000000001</v>
       </c>
       <c r="K36">
-        <v>958</v>
+        <v>887</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D37">
-        <v>79.903999999999996</v>
+        <v>78.959999999999994</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G37">
-        <v>2.96</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="H37">
-        <v>11.813800000000001</v>
+        <v>9.7523999999999997</v>
       </c>
       <c r="I37" s="1">
-        <v>3.12</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="J37">
-        <v>266.05</v>
+        <v>494.15</v>
       </c>
       <c r="K37">
-        <v>332</v>
+        <v>958</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D38">
-        <v>83.798000000000002</v>
+        <v>79.903999999999996</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="G38">
+        <v>2.96</v>
       </c>
       <c r="H38">
-        <v>13.999599999999999</v>
+        <v>11.813800000000001</v>
       </c>
       <c r="I38" s="1">
-        <v>3.7299999999999998E-3</v>
+        <v>3.12</v>
       </c>
       <c r="J38">
-        <v>115.93</v>
+        <v>266.05</v>
       </c>
       <c r="K38">
-        <v>119.93</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D39">
-        <v>85.468000000000004</v>
+        <v>83.798000000000002</v>
       </c>
       <c r="E39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39">
-        <v>0.82</v>
+        <v>14</v>
       </c>
       <c r="H39">
-        <v>4.1771000000000003</v>
+        <v>13.999599999999999</v>
       </c>
       <c r="I39" s="1">
-        <v>1.53</v>
+        <v>3.7299999999999998E-3</v>
       </c>
       <c r="J39">
-        <v>312.79000000000002</v>
+        <v>115.93</v>
       </c>
       <c r="K39">
-        <v>961</v>
+        <v>119.93</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D40">
-        <v>87.62</v>
+        <v>85.468000000000004</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G40">
-        <v>0.95</v>
+        <v>0.82</v>
       </c>
       <c r="H40">
-        <v>5.6948999999999996</v>
+        <v>4.1771000000000003</v>
       </c>
       <c r="I40" s="1">
-        <v>2.64</v>
+        <v>1.53</v>
       </c>
       <c r="J40">
-        <v>1042.1500000000001</v>
+        <v>312.79000000000002</v>
       </c>
       <c r="K40">
-        <v>1655</v>
+        <v>961</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41">
-        <v>88.906000000000006</v>
+        <v>87.62</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="G41">
-        <v>1.22</v>
+        <v>0.95</v>
       </c>
       <c r="H41">
-        <v>6.2172999999999998</v>
+        <v>5.6948999999999996</v>
       </c>
       <c r="I41" s="1">
-        <v>4.47</v>
+        <v>2.64</v>
       </c>
       <c r="J41">
-        <v>1799.15</v>
+        <v>1042.1500000000001</v>
       </c>
       <c r="K41">
-        <v>3609</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42">
-        <v>91.224000000000004</v>
+        <v>88.906000000000006</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
@@ -2906,33 +2909,33 @@
         <v>57</v>
       </c>
       <c r="G42">
-        <v>1.33</v>
+        <v>1.22</v>
       </c>
       <c r="H42">
-        <v>6.6338999999999997</v>
+        <v>6.2172999999999998</v>
       </c>
       <c r="I42" s="1">
-        <v>6.51</v>
+        <v>4.47</v>
       </c>
       <c r="J42">
-        <v>2125.15</v>
+        <v>1799.15</v>
       </c>
       <c r="K42">
-        <v>4682</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D43">
-        <v>92.906000000000006</v>
+        <v>91.224000000000004</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -2941,33 +2944,33 @@
         <v>57</v>
       </c>
       <c r="G43">
-        <v>1.6</v>
+        <v>1.33</v>
       </c>
       <c r="H43">
-        <v>6.7588999999999997</v>
+        <v>6.6338999999999997</v>
       </c>
       <c r="I43" s="1">
-        <v>8.57</v>
+        <v>6.51</v>
       </c>
       <c r="J43">
-        <v>2741.15</v>
+        <v>2125.15</v>
       </c>
       <c r="K43">
-        <v>5017</v>
+        <v>4682</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D44">
-        <v>95.96</v>
+        <v>92.906000000000006</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -2976,33 +2979,33 @@
         <v>57</v>
       </c>
       <c r="G44">
-        <v>2.16</v>
+        <v>1.6</v>
       </c>
       <c r="H44">
-        <v>7.0923999999999996</v>
+        <v>6.7588999999999997</v>
       </c>
       <c r="I44" s="1">
-        <v>10.199999999999999</v>
+        <v>8.57</v>
       </c>
       <c r="J44">
-        <v>2890.15</v>
+        <v>2741.15</v>
       </c>
       <c r="K44">
-        <v>4912</v>
+        <v>5017</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45">
-        <v>98</v>
+        <v>95.96</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -3011,33 +3014,33 @@
         <v>57</v>
       </c>
       <c r="G45">
-        <v>1.9</v>
+        <v>2.16</v>
       </c>
       <c r="H45">
-        <v>7.28</v>
+        <v>7.0923999999999996</v>
       </c>
       <c r="I45" s="1">
-        <v>11.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="J45">
-        <v>2473.15</v>
+        <v>2890.15</v>
       </c>
       <c r="K45">
-        <v>5150</v>
+        <v>4912</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D46">
-        <v>101.07</v>
+        <v>98</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -3046,33 +3049,33 @@
         <v>57</v>
       </c>
       <c r="G46">
-        <v>2.2000000000000002</v>
+        <v>1.9</v>
       </c>
       <c r="H46">
-        <v>7.3605</v>
+        <v>7.28</v>
       </c>
       <c r="I46" s="1">
-        <v>12.4</v>
+        <v>11.5</v>
       </c>
       <c r="J46">
-        <v>2523.15</v>
+        <v>2473.15</v>
       </c>
       <c r="K46">
-        <v>4423</v>
+        <v>5150</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D47">
-        <v>102.90600000000001</v>
+        <v>101.07</v>
       </c>
       <c r="E47" t="b">
         <v>1</v>
@@ -3081,33 +3084,33 @@
         <v>57</v>
       </c>
       <c r="G47">
-        <v>2.2799999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H47">
-        <v>7.4588999999999999</v>
+        <v>7.3605</v>
       </c>
       <c r="I47" s="1">
         <v>12.4</v>
       </c>
       <c r="J47">
-        <v>2239.15</v>
+        <v>2523.15</v>
       </c>
       <c r="K47">
-        <v>3968</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D48">
-        <v>106.42</v>
+        <v>102.90600000000001</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
@@ -3116,33 +3119,33 @@
         <v>57</v>
       </c>
       <c r="G48">
-        <v>2.2000000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="H48">
-        <v>8.3369</v>
+        <v>7.4588999999999999</v>
       </c>
       <c r="I48" s="1">
-        <v>12</v>
+        <v>12.4</v>
       </c>
       <c r="J48">
-        <v>1825.15</v>
+        <v>2239.15</v>
       </c>
       <c r="K48">
-        <v>3236</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D49">
-        <v>107.86799999999999</v>
+        <v>106.42</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
@@ -3151,33 +3154,33 @@
         <v>57</v>
       </c>
       <c r="G49">
-        <v>1.93</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H49">
-        <v>7.5762</v>
+        <v>8.3369</v>
       </c>
       <c r="I49" s="1">
-        <v>10.5</v>
+        <v>12</v>
       </c>
       <c r="J49">
-        <v>1234.1500000000001</v>
+        <v>1825.15</v>
       </c>
       <c r="K49">
-        <v>2435</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D50">
-        <v>112.411</v>
+        <v>107.86799999999999</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -3186,68 +3189,68 @@
         <v>57</v>
       </c>
       <c r="G50">
-        <v>1.69</v>
+        <v>1.93</v>
       </c>
       <c r="H50">
-        <v>8.9938000000000002</v>
+        <v>7.5762</v>
       </c>
       <c r="I50" s="1">
-        <v>8.69</v>
+        <v>10.5</v>
       </c>
       <c r="J50">
-        <v>594.33000000000004</v>
+        <v>1234.1500000000001</v>
       </c>
       <c r="K50">
-        <v>1040</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D51">
-        <v>114.818</v>
+        <v>112.411</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G51">
-        <v>1.78</v>
+        <v>1.69</v>
       </c>
       <c r="H51">
-        <v>5.7864000000000004</v>
+        <v>8.9938000000000002</v>
       </c>
       <c r="I51" s="1">
-        <v>7.31</v>
+        <v>8.69</v>
       </c>
       <c r="J51">
-        <v>429.91</v>
+        <v>594.33000000000004</v>
       </c>
       <c r="K51">
-        <v>2345</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D52">
-        <v>118.71</v>
+        <v>114.818</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -3256,68 +3259,68 @@
         <v>4</v>
       </c>
       <c r="G52">
-        <v>1.96</v>
+        <v>1.78</v>
       </c>
       <c r="H52">
-        <v>7.3438999999999997</v>
+        <v>5.7864000000000004</v>
       </c>
       <c r="I52" s="1">
-        <v>7.29</v>
+        <v>7.31</v>
       </c>
       <c r="J52">
-        <v>505.21</v>
+        <v>429.91</v>
       </c>
       <c r="K52">
-        <v>2875</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D53">
-        <v>121.76</v>
+        <v>118.71</v>
       </c>
       <c r="E53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G53">
-        <v>2.0499999999999998</v>
+        <v>1.96</v>
       </c>
       <c r="H53">
-        <v>8.6083999999999996</v>
+        <v>7.3438999999999997</v>
       </c>
       <c r="I53" s="1">
-        <v>6.69</v>
+        <v>7.29</v>
       </c>
       <c r="J53">
-        <v>904.05</v>
+        <v>505.21</v>
       </c>
       <c r="K53">
-        <v>1860</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D54">
-        <v>127.6</v>
+        <v>121.76</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -3326,205 +3329,205 @@
         <v>23</v>
       </c>
       <c r="G54">
-        <v>2.1</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H54">
-        <v>9.0096000000000007</v>
+        <v>8.6083999999999996</v>
       </c>
       <c r="I54" s="1">
-        <v>6.23</v>
+        <v>6.69</v>
       </c>
       <c r="J54">
-        <v>722.8</v>
+        <v>904.05</v>
       </c>
       <c r="K54">
-        <v>1261</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D55">
-        <v>126.904</v>
+        <v>127.6</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G55">
-        <v>2.66</v>
+        <v>2.1</v>
       </c>
       <c r="H55">
-        <v>10.4513</v>
+        <v>9.0096000000000007</v>
       </c>
       <c r="I55" s="1">
-        <v>4.93</v>
+        <v>6.23</v>
       </c>
       <c r="J55">
-        <v>386.65</v>
+        <v>722.8</v>
       </c>
       <c r="K55">
-        <v>457.4</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D56">
-        <v>131.29300000000001</v>
+        <v>126.904</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="G56">
+        <v>2.66</v>
       </c>
       <c r="H56">
-        <v>12.129799999999999</v>
+        <v>10.4513</v>
       </c>
       <c r="I56" s="1">
-        <v>5.8900000000000003E-3</v>
+        <v>4.93</v>
       </c>
       <c r="J56">
-        <v>161.44999999999999</v>
+        <v>386.65</v>
       </c>
       <c r="K56">
-        <v>165.03</v>
+        <v>457.4</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D57">
-        <v>132.905</v>
+        <v>131.29300000000001</v>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57">
-        <v>0.79</v>
+        <v>14</v>
       </c>
       <c r="H57">
-        <v>3.8938999999999999</v>
+        <v>12.129799999999999</v>
       </c>
       <c r="I57" s="1">
-        <v>1.87</v>
+        <v>5.8900000000000003E-3</v>
       </c>
       <c r="J57">
-        <v>301.7</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="K57">
-        <v>944</v>
+        <v>165.03</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D58">
-        <v>137.327</v>
+        <v>132.905</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G58">
-        <v>0.89</v>
+        <v>0.79</v>
       </c>
       <c r="H58">
-        <v>5.2117000000000004</v>
+        <v>3.8938999999999999</v>
       </c>
       <c r="I58" s="1">
-        <v>3.59</v>
+        <v>1.87</v>
       </c>
       <c r="J58">
-        <v>1002.15</v>
+        <v>301.7</v>
       </c>
       <c r="K58">
-        <v>2170</v>
+        <v>944</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D59">
-        <v>138.905</v>
+        <v>137.327</v>
       </c>
       <c r="E59" t="b">
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="G59">
-        <v>1.1000000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="H59">
-        <v>5.5769000000000002</v>
+        <v>5.2117000000000004</v>
       </c>
       <c r="I59" s="1">
-        <v>6.15</v>
+        <v>3.59</v>
       </c>
       <c r="J59">
-        <v>1193.1500000000001</v>
+        <v>1002.15</v>
       </c>
       <c r="K59">
-        <v>3737</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C60" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D60">
-        <v>140.11600000000001</v>
+        <v>138.905</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -3533,33 +3536,33 @@
         <v>130</v>
       </c>
       <c r="G60">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H60">
-        <v>5.5387000000000004</v>
+        <v>5.5769000000000002</v>
       </c>
       <c r="I60" s="1">
-        <v>6.77</v>
+        <v>6.15</v>
       </c>
       <c r="J60">
-        <v>1071.1500000000001</v>
+        <v>1193.1500000000001</v>
       </c>
       <c r="K60">
-        <v>3716</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D61">
-        <v>140.90799999999999</v>
+        <v>140.11600000000001</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -3568,33 +3571,33 @@
         <v>130</v>
       </c>
       <c r="G61">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H61">
-        <v>5.4729999999999999</v>
+        <v>5.5387000000000004</v>
       </c>
       <c r="I61" s="1">
         <v>6.77</v>
       </c>
       <c r="J61">
-        <v>1204.1500000000001</v>
+        <v>1071.1500000000001</v>
       </c>
       <c r="K61">
-        <v>3793</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D62">
-        <v>144.24199999999999</v>
+        <v>140.90799999999999</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -3603,33 +3606,33 @@
         <v>130</v>
       </c>
       <c r="G62">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H62">
-        <v>5.5250000000000004</v>
+        <v>5.4729999999999999</v>
       </c>
       <c r="I62" s="1">
-        <v>7.01</v>
+        <v>6.77</v>
       </c>
       <c r="J62">
-        <v>1289.1500000000001</v>
+        <v>1204.1500000000001</v>
       </c>
       <c r="K62">
-        <v>3347</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D63">
-        <v>145</v>
+        <v>144.24199999999999</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -3638,33 +3641,33 @@
         <v>130</v>
       </c>
       <c r="G63">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H63">
-        <v>5.5819999999999999</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="I63" s="1">
-        <v>7.26</v>
+        <v>7.01</v>
       </c>
       <c r="J63">
-        <v>1204.1500000000001</v>
+        <v>1289.1500000000001</v>
       </c>
       <c r="K63">
-        <v>3273</v>
+        <v>3347</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D64">
-        <v>150.36000000000001</v>
+        <v>145</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -3673,33 +3676,33 @@
         <v>130</v>
       </c>
       <c r="G64">
-        <v>1.17</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H64">
-        <v>5.6436999999999999</v>
+        <v>5.5819999999999999</v>
       </c>
       <c r="I64" s="1">
-        <v>7.52</v>
+        <v>7.26</v>
       </c>
       <c r="J64">
-        <v>1345.15</v>
+        <v>1204.1500000000001</v>
       </c>
       <c r="K64">
-        <v>2067</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D65">
-        <v>151.964</v>
+        <v>150.36000000000001</v>
       </c>
       <c r="E65" t="b">
         <v>1</v>
@@ -3708,33 +3711,33 @@
         <v>130</v>
       </c>
       <c r="G65">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
       <c r="H65">
-        <v>5.6703999999999999</v>
+        <v>5.6436999999999999</v>
       </c>
       <c r="I65" s="1">
-        <v>5.24</v>
+        <v>7.52</v>
       </c>
       <c r="J65">
-        <v>1095.1500000000001</v>
+        <v>1345.15</v>
       </c>
       <c r="K65">
-        <v>1802</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D66">
-        <v>157.25</v>
+        <v>151.964</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
@@ -3746,30 +3749,30 @@
         <v>1.2</v>
       </c>
       <c r="H66">
-        <v>6.1501000000000001</v>
+        <v>5.6703999999999999</v>
       </c>
       <c r="I66" s="1">
-        <v>7.9</v>
+        <v>5.24</v>
       </c>
       <c r="J66">
-        <v>1585.15</v>
+        <v>1095.1500000000001</v>
       </c>
       <c r="K66">
-        <v>3546</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D67">
-        <v>158.92500000000001</v>
+        <v>157.25</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
@@ -3781,30 +3784,30 @@
         <v>1.2</v>
       </c>
       <c r="H67">
-        <v>5.8638000000000003</v>
+        <v>6.1501000000000001</v>
       </c>
       <c r="I67" s="1">
-        <v>8.23</v>
+        <v>7.9</v>
       </c>
       <c r="J67">
-        <v>1630.15</v>
+        <v>1585.15</v>
       </c>
       <c r="K67">
-        <v>3503</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D68">
-        <v>162.5</v>
+        <v>158.92500000000001</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
@@ -3813,33 +3816,33 @@
         <v>130</v>
       </c>
       <c r="G68">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="H68">
-        <v>5.9389000000000003</v>
+        <v>5.8638000000000003</v>
       </c>
       <c r="I68" s="1">
-        <v>8.5500000000000007</v>
+        <v>8.23</v>
       </c>
       <c r="J68">
-        <v>1680.15</v>
+        <v>1630.15</v>
       </c>
       <c r="K68">
-        <v>2840</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D69">
-        <v>164.93</v>
+        <v>162.5</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
@@ -3848,33 +3851,33 @@
         <v>130</v>
       </c>
       <c r="G69">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="H69">
-        <v>6.0214999999999996</v>
+        <v>5.9389000000000003</v>
       </c>
       <c r="I69" s="1">
-        <v>8.8000000000000007</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="J69">
-        <v>1743.15</v>
+        <v>1680.15</v>
       </c>
       <c r="K69">
-        <v>2993</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D70">
-        <v>167.25899999999999</v>
+        <v>164.93</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
@@ -3883,33 +3886,33 @@
         <v>130</v>
       </c>
       <c r="G70">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="H70">
-        <v>6.1077000000000004</v>
+        <v>6.0214999999999996</v>
       </c>
       <c r="I70" s="1">
-        <v>9.07</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J70">
-        <v>1795.15</v>
+        <v>1743.15</v>
       </c>
       <c r="K70">
-        <v>3503</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D71">
-        <v>168.934</v>
+        <v>167.25899999999999</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -3918,33 +3921,33 @@
         <v>130</v>
       </c>
       <c r="G71">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="H71">
-        <v>6.1843000000000004</v>
+        <v>6.1077000000000004</v>
       </c>
       <c r="I71" s="1">
-        <v>9.32</v>
+        <v>9.07</v>
       </c>
       <c r="J71">
-        <v>1818.15</v>
+        <v>1795.15</v>
       </c>
       <c r="K71">
-        <v>2223</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D72">
-        <v>173.054</v>
+        <v>168.934</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
@@ -3953,33 +3956,33 @@
         <v>130</v>
       </c>
       <c r="G72">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="H72">
-        <v>6.2542</v>
+        <v>6.1843000000000004</v>
       </c>
       <c r="I72" s="1">
-        <v>6.97</v>
+        <v>9.32</v>
       </c>
       <c r="J72">
-        <v>1097.1500000000001</v>
+        <v>1818.15</v>
       </c>
       <c r="K72">
-        <v>1469</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D73">
-        <v>174.96700000000001</v>
+        <v>173.054</v>
       </c>
       <c r="E73" t="b">
         <v>1</v>
@@ -3988,68 +3991,68 @@
         <v>130</v>
       </c>
       <c r="G73">
-        <v>1.27</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H73">
-        <v>5.4259000000000004</v>
+        <v>6.2542</v>
       </c>
       <c r="I73" s="1">
-        <v>9.84</v>
+        <v>6.97</v>
       </c>
       <c r="J73">
-        <v>1936.15</v>
+        <v>1097.1500000000001</v>
       </c>
       <c r="K73">
-        <v>3675</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D74">
-        <v>178.49</v>
+        <v>174.96700000000001</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="G74">
-        <v>1.3</v>
+        <v>1.27</v>
       </c>
       <c r="H74">
-        <v>6.8250999999999999</v>
+        <v>5.4259000000000004</v>
       </c>
       <c r="I74" s="1">
-        <v>13.3</v>
+        <v>9.84</v>
       </c>
       <c r="J74">
-        <v>2500.15</v>
+        <v>1936.15</v>
       </c>
       <c r="K74">
-        <v>4876</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D75">
-        <v>180.94800000000001</v>
+        <v>178.49</v>
       </c>
       <c r="E75" t="b">
         <v>1</v>
@@ -4058,33 +4061,33 @@
         <v>57</v>
       </c>
       <c r="G75">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="H75">
-        <v>7.5495999999999999</v>
+        <v>6.8250999999999999</v>
       </c>
       <c r="I75" s="1">
-        <v>16.7</v>
+        <v>13.3</v>
       </c>
       <c r="J75">
-        <v>3269.15</v>
+        <v>2500.15</v>
       </c>
       <c r="K75">
-        <v>5731</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C76" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D76">
-        <v>183.84</v>
+        <v>180.94800000000001</v>
       </c>
       <c r="E76" t="b">
         <v>1</v>
@@ -4093,33 +4096,33 @@
         <v>57</v>
       </c>
       <c r="G76">
-        <v>2.36</v>
+        <v>1.5</v>
       </c>
       <c r="H76">
-        <v>7.8639999999999999</v>
+        <v>7.5495999999999999</v>
       </c>
       <c r="I76" s="1">
-        <v>19.3</v>
+        <v>16.7</v>
       </c>
       <c r="J76">
-        <v>3680.15</v>
+        <v>3269.15</v>
       </c>
       <c r="K76">
-        <v>5828</v>
+        <v>5731</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D77">
-        <v>186.20699999999999</v>
+        <v>183.84</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -4128,33 +4131,33 @@
         <v>57</v>
       </c>
       <c r="G77">
-        <v>1.9</v>
+        <v>2.36</v>
       </c>
       <c r="H77">
-        <v>7.8334999999999999</v>
+        <v>7.8639999999999999</v>
       </c>
       <c r="I77" s="1">
-        <v>21</v>
+        <v>19.3</v>
       </c>
       <c r="J77">
-        <v>3453.15</v>
+        <v>3680.15</v>
       </c>
       <c r="K77">
-        <v>5869</v>
+        <v>5828</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D78">
-        <v>190.23</v>
+        <v>186.20699999999999</v>
       </c>
       <c r="E78" t="b">
         <v>1</v>
@@ -4163,33 +4166,33 @@
         <v>57</v>
       </c>
       <c r="G78">
-        <v>2.2000000000000002</v>
+        <v>1.9</v>
       </c>
       <c r="H78">
-        <v>8.4382000000000001</v>
+        <v>7.8334999999999999</v>
       </c>
       <c r="I78" s="1">
-        <v>22.6</v>
+        <v>21</v>
       </c>
       <c r="J78">
-        <v>3300.15</v>
+        <v>3453.15</v>
       </c>
       <c r="K78">
-        <v>5285</v>
+        <v>5869</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D79">
-        <v>192.21700000000001</v>
+        <v>190.23</v>
       </c>
       <c r="E79" t="b">
         <v>1</v>
@@ -4201,30 +4204,30 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H79">
-        <v>8.9670000000000005</v>
+        <v>8.4382000000000001</v>
       </c>
       <c r="I79" s="1">
         <v>22.6</v>
       </c>
       <c r="J79">
-        <v>2716.15</v>
+        <v>3300.15</v>
       </c>
       <c r="K79">
-        <v>4701</v>
+        <v>5285</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D80">
-        <v>195.084</v>
+        <v>192.21700000000001</v>
       </c>
       <c r="E80" t="b">
         <v>1</v>
@@ -4233,33 +4236,33 @@
         <v>57</v>
       </c>
       <c r="G80">
-        <v>2.2799999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H80">
-        <v>8.9587000000000003</v>
+        <v>8.9670000000000005</v>
       </c>
       <c r="I80" s="1">
-        <v>21.5</v>
+        <v>22.6</v>
       </c>
       <c r="J80">
-        <v>2045.15</v>
+        <v>2716.15</v>
       </c>
       <c r="K80">
-        <v>4098</v>
+        <v>4701</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D81">
-        <v>196.96700000000001</v>
+        <v>195.084</v>
       </c>
       <c r="E81" t="b">
         <v>1</v>
@@ -4268,33 +4271,33 @@
         <v>57</v>
       </c>
       <c r="G81">
-        <v>2.54</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="H81">
-        <v>9.2255000000000003</v>
+        <v>8.9587000000000003</v>
       </c>
       <c r="I81" s="1">
-        <v>19.3</v>
+        <v>21.5</v>
       </c>
       <c r="J81">
-        <v>1337.73</v>
+        <v>2045.15</v>
       </c>
       <c r="K81">
-        <v>3129</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D82">
-        <v>200.59</v>
+        <v>196.96700000000001</v>
       </c>
       <c r="E82" t="b">
         <v>1</v>
@@ -4303,68 +4306,68 @@
         <v>57</v>
       </c>
       <c r="G82">
-        <v>2</v>
+        <v>2.54</v>
       </c>
       <c r="H82">
-        <v>10.4375</v>
+        <v>9.2255000000000003</v>
       </c>
       <c r="I82" s="1">
-        <v>13.5</v>
+        <v>19.3</v>
       </c>
       <c r="J82">
-        <v>234.43</v>
+        <v>1337.73</v>
       </c>
       <c r="K82">
-        <v>630</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D83">
-        <v>204.38300000000001</v>
+        <v>200.59</v>
       </c>
       <c r="E83" t="b">
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G83">
-        <v>2.04</v>
+        <v>2</v>
       </c>
       <c r="H83">
-        <v>6.1082000000000001</v>
+        <v>10.4375</v>
       </c>
       <c r="I83" s="1">
-        <v>11.9</v>
+        <v>13.5</v>
       </c>
       <c r="J83">
-        <v>577.15</v>
+        <v>234.43</v>
       </c>
       <c r="K83">
-        <v>1746</v>
+        <v>630</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D84">
-        <v>207.2</v>
+        <v>204.38300000000001</v>
       </c>
       <c r="E84" t="b">
         <v>1</v>
@@ -4373,33 +4376,33 @@
         <v>4</v>
       </c>
       <c r="G84">
-        <v>2.33</v>
+        <v>2.04</v>
       </c>
       <c r="H84">
-        <v>7.4166999999999996</v>
+        <v>6.1082000000000001</v>
       </c>
       <c r="I84" s="1">
-        <v>11.3</v>
+        <v>11.9</v>
       </c>
       <c r="J84">
-        <v>600.75</v>
+        <v>577.15</v>
       </c>
       <c r="K84">
-        <v>2022</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C85" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D85">
-        <v>208.98</v>
+        <v>207.2</v>
       </c>
       <c r="E85" t="b">
         <v>1</v>
@@ -4408,65 +4411,65 @@
         <v>4</v>
       </c>
       <c r="G85">
-        <v>2.02</v>
+        <v>2.33</v>
       </c>
       <c r="H85">
-        <v>7.2855999999999996</v>
+        <v>7.4166999999999996</v>
       </c>
       <c r="I85" s="1">
-        <v>9.81</v>
+        <v>11.3</v>
       </c>
       <c r="J85">
-        <v>544.66999999999996</v>
+        <v>600.75</v>
       </c>
       <c r="K85">
-        <v>1837</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D86">
-        <v>210</v>
+        <v>208.98</v>
       </c>
       <c r="E86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="H86">
-        <v>8.4169999999999998</v>
+        <v>7.2855999999999996</v>
       </c>
       <c r="I86" s="1">
-        <v>9.32</v>
+        <v>9.81</v>
       </c>
       <c r="J86">
-        <v>527.15</v>
+        <v>544.66999999999996</v>
       </c>
       <c r="K86">
-        <v>1235</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C87" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D87">
         <v>210</v>
@@ -4475,138 +4478,138 @@
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G87">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H87">
-        <v>9.3000000000000007</v>
+        <v>8.4169999999999998</v>
       </c>
       <c r="I87" s="1">
-        <v>7</v>
+        <v>9.32</v>
       </c>
       <c r="J87">
-        <v>575.15</v>
+        <v>527.15</v>
       </c>
       <c r="K87">
-        <v>610</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D88">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="G88">
+        <v>2.2000000000000002</v>
       </c>
       <c r="H88">
-        <v>10.7485</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I88" s="1">
-        <v>9.7300000000000008E-3</v>
+        <v>7</v>
       </c>
       <c r="J88">
-        <v>202.15</v>
+        <v>575.15</v>
       </c>
       <c r="K88">
-        <v>211.3</v>
+        <v>610</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D89">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>20</v>
-      </c>
-      <c r="G89">
-        <v>0.7</v>
+        <v>17</v>
       </c>
       <c r="H89">
-        <v>4.0727000000000002</v>
+        <v>10.7485</v>
       </c>
       <c r="I89" s="1">
-        <v>1.87</v>
+        <v>9.7300000000000008E-3</v>
       </c>
       <c r="J89">
-        <v>300.14999999999998</v>
+        <v>202.15</v>
       </c>
       <c r="K89">
-        <v>950</v>
+        <v>211.3</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C90" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D90">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E90" t="b">
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>193</v>
+        <v>20</v>
       </c>
       <c r="G90">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="H90">
-        <v>5.2784000000000004</v>
+        <v>4.0727000000000002</v>
       </c>
       <c r="I90" s="1">
-        <v>5.5</v>
+        <v>1.87</v>
       </c>
       <c r="J90">
-        <v>973.15</v>
+        <v>300.14999999999998</v>
       </c>
       <c r="K90">
-        <v>2010</v>
+        <v>950</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D91">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E91" t="b">
         <v>1</v>
@@ -4615,33 +4618,33 @@
         <v>193</v>
       </c>
       <c r="G91">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H91">
-        <v>5.17</v>
+        <v>5.2784000000000004</v>
       </c>
       <c r="I91" s="1">
-        <v>10.1</v>
+        <v>5.5</v>
       </c>
       <c r="J91">
-        <v>1323.15</v>
+        <v>973.15</v>
       </c>
       <c r="K91">
-        <v>3471</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C92" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D92">
-        <v>232.03800000000001</v>
+        <v>227</v>
       </c>
       <c r="E92" t="b">
         <v>1</v>
@@ -4650,33 +4653,33 @@
         <v>193</v>
       </c>
       <c r="G92">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H92">
-        <v>6.3067000000000002</v>
+        <v>5.17</v>
       </c>
       <c r="I92" s="1">
-        <v>11.7</v>
+        <v>10.1</v>
       </c>
       <c r="J92">
-        <v>2028.15</v>
+        <v>1323.15</v>
       </c>
       <c r="K92">
-        <v>5061</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C93" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D93">
-        <v>231.036</v>
+        <v>232.03800000000001</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -4685,33 +4688,33 @@
         <v>193</v>
       </c>
       <c r="G93">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="H93">
-        <v>5.89</v>
+        <v>6.3067000000000002</v>
       </c>
       <c r="I93" s="1">
-        <v>15.4</v>
+        <v>11.7</v>
       </c>
       <c r="J93">
-        <v>1873.15</v>
+        <v>2028.15</v>
       </c>
       <c r="K93">
-        <v>4300</v>
+        <v>5061</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C94" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D94">
-        <v>238.029</v>
+        <v>231.036</v>
       </c>
       <c r="E94" t="b">
         <v>1</v>
@@ -4720,33 +4723,33 @@
         <v>193</v>
       </c>
       <c r="G94">
-        <v>1.38</v>
+        <v>1.5</v>
       </c>
       <c r="H94">
-        <v>6.1940999999999997</v>
+        <v>5.89</v>
       </c>
       <c r="I94" s="1">
-        <v>19</v>
+        <v>15.4</v>
       </c>
       <c r="J94">
-        <v>1405.15</v>
+        <v>1873.15</v>
       </c>
       <c r="K94">
-        <v>4404</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C95" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D95">
-        <v>237</v>
+        <v>238.029</v>
       </c>
       <c r="E95" t="b">
         <v>1</v>
@@ -4755,33 +4758,33 @@
         <v>193</v>
       </c>
       <c r="G95">
-        <v>1.36</v>
+        <v>1.38</v>
       </c>
       <c r="H95">
-        <v>6.2656999999999998</v>
+        <v>6.1940999999999997</v>
       </c>
       <c r="I95" s="1">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="J95">
-        <v>913.15</v>
+        <v>1405.15</v>
       </c>
       <c r="K95">
-        <v>4273</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C96" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D96">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E96" t="b">
         <v>1</v>
@@ -4790,33 +4793,33 @@
         <v>193</v>
       </c>
       <c r="G96">
-        <v>1.28</v>
+        <v>1.36</v>
       </c>
       <c r="H96">
-        <v>6.0262000000000002</v>
+        <v>6.2656999999999998</v>
       </c>
       <c r="I96" s="1">
-        <v>19.8</v>
+        <v>20.5</v>
       </c>
       <c r="J96">
         <v>913.15</v>
       </c>
       <c r="K96">
-        <v>3501</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C97" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D97">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E97" t="b">
         <v>1</v>
@@ -4825,33 +4828,33 @@
         <v>193</v>
       </c>
       <c r="G97">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="H97">
-        <v>5.9737999999999998</v>
+        <v>6.0262000000000002</v>
       </c>
       <c r="I97" s="1">
-        <v>13.7</v>
+        <v>19.8</v>
       </c>
       <c r="J97">
-        <v>1267.1500000000001</v>
+        <v>913.15</v>
       </c>
       <c r="K97">
-        <v>2880</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C98" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D98">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
@@ -4863,27 +4866,27 @@
         <v>1.3</v>
       </c>
       <c r="H98">
-        <v>5.9915000000000003</v>
+        <v>5.9737999999999998</v>
       </c>
       <c r="I98" s="1">
-        <v>13.5</v>
+        <v>13.7</v>
       </c>
       <c r="J98">
-        <v>1340.15</v>
+        <v>1267.1500000000001</v>
       </c>
       <c r="K98">
-        <v>3383</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C99" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D99">
         <v>247</v>
@@ -4898,30 +4901,30 @@
         <v>1.3</v>
       </c>
       <c r="H99">
-        <v>6.1978999999999997</v>
+        <v>5.9915000000000003</v>
       </c>
       <c r="I99" s="1">
-        <v>14.8</v>
+        <v>13.5</v>
       </c>
       <c r="J99">
-        <v>1259.1500000000001</v>
+        <v>1340.15</v>
       </c>
       <c r="K99">
-        <v>983</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C100" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D100">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E100" t="b">
         <v>1</v>
@@ -4933,30 +4936,30 @@
         <v>1.3</v>
       </c>
       <c r="H100">
-        <v>6.2816999999999998</v>
+        <v>6.1978999999999997</v>
       </c>
       <c r="I100" s="1">
-        <v>15.1</v>
+        <v>14.8</v>
       </c>
       <c r="J100">
-        <v>1925.15</v>
+        <v>1259.1500000000001</v>
       </c>
       <c r="K100">
-        <v>1173</v>
+        <v>983</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C101" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D101">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -4968,27 +4971,30 @@
         <v>1.3</v>
       </c>
       <c r="H101">
-        <v>6.42</v>
+        <v>6.2816999999999998</v>
       </c>
       <c r="I101" s="1">
-        <v>13.5</v>
+        <v>15.1</v>
       </c>
       <c r="J101">
-        <v>1133.1500000000001</v>
+        <v>1925.15</v>
+      </c>
+      <c r="K101">
+        <v>1173</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C102" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D102">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
@@ -5000,21 +5006,27 @@
         <v>1.3</v>
       </c>
       <c r="H102">
-        <v>6.5</v>
+        <v>6.42</v>
+      </c>
+      <c r="I102" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J102">
+        <v>1133.1500000000001</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C103" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D103">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E103" t="b">
         <v>1</v>
@@ -5026,21 +5038,21 @@
         <v>1.3</v>
       </c>
       <c r="H103">
-        <v>6.58</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C104" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D104">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E104" t="b">
         <v>1</v>
@@ -5052,21 +5064,21 @@
         <v>1.3</v>
       </c>
       <c r="H104">
-        <v>6.65</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C105" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D105">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E105" t="b">
         <v>1</v>
@@ -5074,42 +5086,45 @@
       <c r="F105" t="s">
         <v>193</v>
       </c>
+      <c r="G105">
+        <v>1.3</v>
+      </c>
+      <c r="H105">
+        <v>6.65</v>
+      </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C106" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D106">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E106" t="b">
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>226</v>
-      </c>
-      <c r="I106" s="1">
-        <v>18.100000000000001</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C107" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D107">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E107" t="b">
         <v>1</v>
@@ -5118,21 +5133,21 @@
         <v>226</v>
       </c>
       <c r="I107" s="1">
-        <v>39</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C108" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D108">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E108" t="b">
         <v>1</v>
@@ -5141,21 +5156,21 @@
         <v>226</v>
       </c>
       <c r="I108" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C109" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D109">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E109" t="b">
         <v>1</v>
@@ -5164,21 +5179,21 @@
         <v>226</v>
       </c>
       <c r="I109" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C110" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D110">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E110" t="b">
         <v>1</v>
@@ -5187,21 +5202,21 @@
         <v>226</v>
       </c>
       <c r="I110" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C111" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D111">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E111" t="b">
         <v>1</v>
@@ -5210,21 +5225,21 @@
         <v>226</v>
       </c>
       <c r="I111" s="1">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C112" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D112">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E112" t="b">
         <v>1</v>
@@ -5232,19 +5247,22 @@
       <c r="F112" t="s">
         <v>226</v>
       </c>
+      <c r="I112" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C113" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D113">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E113" t="b">
         <v>1</v>
@@ -5255,16 +5273,16 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C114" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D114">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="E114" t="b">
         <v>1</v>
@@ -5275,112 +5293,132 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C115" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D115">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E115" t="b">
         <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C116" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D116">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E116" t="b">
         <v>1</v>
-      </c>
-      <c r="F116" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D117">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E117" t="b">
         <v>1</v>
+      </c>
+      <c r="F117" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C118" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D118">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E118" t="b">
         <v>1</v>
-      </c>
-      <c r="F118" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C119" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D119">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E119" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C120" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D120">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E120" t="b">
         <v>0</v>
       </c>
-      <c r="F120" t="s">
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121" t="s">
+        <v>253</v>
+      </c>
+      <c r="C121" t="s">
+        <v>254</v>
+      </c>
+      <c r="D121">
+        <v>294</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rococo.carpenter - PeriodicTable compiles fine. We need to define Rococo::IO::ParseTableRows to complete dynamic loading of tables
</commit_message>
<xml_diff>
--- a/tables/periodic-table.xlsx
+++ b/tables/periodic-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4119549D-2003-45B9-AA44-7BE7030AD590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFFB243-4580-4803-A5FE-46BA91391F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
+    <workbookView xWindow="4440" yWindow="5790" windowWidth="21600" windowHeight="9030" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sexcel-Spec" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="303">
   <si>
     <t>AtomicNumber</t>
   </si>
@@ -890,9 +890,6 @@
     <t>Lifetime</t>
   </si>
   <si>
-    <t>Static</t>
-  </si>
-  <si>
     <t>Namespace</t>
   </si>
   <si>
@@ -926,25 +923,28 @@
     <t>$(ROCOCO)</t>
   </si>
   <si>
+    <t>tables\rococo.periodic-table.cpp</t>
+  </si>
+  <si>
+    <t>ElectroNegativity</t>
+  </si>
+  <si>
+    <t>Enum-ElementSymbol</t>
+  </si>
+  <si>
+    <t>Enum-ElementName</t>
+  </si>
+  <si>
+    <t>Int32</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Dynamic</t>
+  </si>
+  <si>
     <t>tables\rococo.periodic-table.h</t>
-  </si>
-  <si>
-    <t>tables\rococo.periodic-table.cpp</t>
-  </si>
-  <si>
-    <t>ElectroNegativity</t>
-  </si>
-  <si>
-    <t>Enum-ElementSymbol</t>
-  </si>
-  <si>
-    <t>Enum-ElementName</t>
-  </si>
-  <si>
-    <t>Int32</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1340,21 +1340,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" t="s">
         <v>285</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>286</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>287</v>
-      </c>
-      <c r="E1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
         <v>274</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B3" t="s">
         <v>274</v>
@@ -1451,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3230684E-8A11-41FB-8526-9EA18FC7052C}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,13 +1471,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D1" t="s">
         <v>268</v>
@@ -1486,7 +1486,7 @@
         <v>269</v>
       </c>
       <c r="F1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G1" t="s">
         <v>268</v>
@@ -1524,7 +1524,7 @@
         <v>270</v>
       </c>
       <c r="G2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -1544,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -5327,6 +5327,9 @@
       <c r="E116" t="b">
         <v>1</v>
       </c>
+      <c r="F116" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
@@ -5364,6 +5367,9 @@
       <c r="E118" t="b">
         <v>1</v>
       </c>
+      <c r="F118" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -5400,6 +5406,9 @@
       </c>
       <c r="E120" t="b">
         <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -5435,8 +5444,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5460,7 +5469,7 @@
         <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5468,7 +5477,7 @@
         <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5476,7 +5485,7 @@
         <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5500,7 +5509,7 @@
         <v>283</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5510,18 +5519,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" t="s">
         <v>289</v>
-      </c>
-      <c r="B9" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" t="s">
         <v>292</v>
-      </c>
-      <c r="B10" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added .sxh generator for the rococo.carpenter application. As this develops this will give us the ability to read carpenter tables using the sexy script language, with the C++ API doing the gruntwork.
</commit_message>
<xml_diff>
--- a/tables/periodic-table.xlsx
+++ b/tables/periodic-table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFFB243-4580-4803-A5FE-46BA91391F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3671DCC1-0D32-4B1B-B8E4-5C458B1A108D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="5790" windowWidth="21600" windowHeight="9030" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sexcel-Spec" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="305">
   <si>
     <t>AtomicNumber</t>
   </si>
@@ -945,6 +945,12 @@
   </si>
   <si>
     <t>tables\rococo.periodic-table.h</t>
+  </si>
+  <si>
+    <t>Sexy Header</t>
+  </si>
+  <si>
+    <t>tables\rococo.tables.test.sxh</t>
   </si>
 </sst>
 </file>
@@ -5442,16 +5448,16 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
   </cols>
@@ -5533,6 +5539,14 @@
         <v>292</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>